<commit_message>
Set PSR to print to one page
</commit_message>
<xml_diff>
--- a/temporary-psr-generation/psr-template.xlsx
+++ b/temporary-psr-generation/psr-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmgiven/Developer/gov.ct/ecis-data-migration/temporary-psr-generation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7893DE8F-F282-EC4B-B93A-73E05E47BE79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2772405-0A28-9145-B71A-463FEB695906}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23020" windowHeight="20520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5480" yWindow="820" windowWidth="23020" windowHeight="20520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PSR" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,17 @@
     <sheet name="Spaces" sheetId="5" r:id="rId4"/>
     <sheet name="Other Details" sheetId="6" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">PSR!$A$1:$Q$43</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -994,6 +999,327 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1082,327 +1408,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1719,10 +1724,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1738,233 +1746,233 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" s="139" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="140"/>
-      <c r="C1" s="140"/>
-      <c r="D1" s="140"/>
-      <c r="E1" s="140"/>
-      <c r="F1" s="140"/>
-      <c r="G1" s="140"/>
-      <c r="H1" s="140"/>
-      <c r="I1" s="140"/>
-      <c r="J1" s="140"/>
-      <c r="K1" s="140"/>
-      <c r="L1" s="140"/>
-      <c r="M1" s="140"/>
-      <c r="N1" s="140"/>
-      <c r="O1" s="140"/>
-      <c r="P1" s="140"/>
-      <c r="Q1" s="141"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="38"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="142" t="s">
+      <c r="A2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="142"/>
-      <c r="C2" s="142"/>
-      <c r="D2" s="142"/>
-      <c r="E2" s="142"/>
-      <c r="F2" s="142"/>
-      <c r="G2" s="142"/>
-      <c r="H2" s="143">
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="40">
         <f>'Other Details'!A2</f>
         <v>0</v>
       </c>
-      <c r="I2" s="143"/>
-      <c r="J2" s="143"/>
-      <c r="K2" s="143"/>
-      <c r="L2" s="143"/>
-      <c r="M2" s="143"/>
-      <c r="N2" s="143"/>
-      <c r="O2" s="143"/>
-      <c r="P2" s="143"/>
-      <c r="Q2" s="144"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="41"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="131"/>
-      <c r="B3" s="132"/>
-      <c r="C3" s="132"/>
-      <c r="D3" s="132"/>
-      <c r="E3" s="132"/>
-      <c r="F3" s="132"/>
-      <c r="G3" s="132"/>
-      <c r="H3" s="132"/>
-      <c r="I3" s="132"/>
-      <c r="J3" s="132"/>
-      <c r="K3" s="132"/>
-      <c r="L3" s="132"/>
-      <c r="M3" s="132"/>
-      <c r="N3" s="132"/>
-      <c r="O3" s="132"/>
-      <c r="P3" s="132"/>
-      <c r="Q3" s="133"/>
+      <c r="A3" s="42"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="43"/>
+      <c r="Q3" s="44"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="145" t="s">
+      <c r="A4" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="146"/>
-      <c r="C4" s="146"/>
-      <c r="D4" s="146"/>
-      <c r="E4" s="146"/>
-      <c r="F4" s="146"/>
-      <c r="G4" s="147">
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="47">
         <f>'Other Details'!B2</f>
         <v>0</v>
       </c>
-      <c r="H4" s="148"/>
-      <c r="I4" s="148"/>
-      <c r="J4" s="148"/>
-      <c r="K4" s="148"/>
-      <c r="L4" s="148"/>
-      <c r="M4" s="149"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="49"/>
       <c r="Q4" s="2"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="145" t="s">
+      <c r="A5" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="146"/>
-      <c r="C5" s="146"/>
-      <c r="D5" s="146"/>
-      <c r="E5" s="146"/>
-      <c r="F5" s="146"/>
-      <c r="G5" s="147">
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="47">
         <f>'Other Details'!C2</f>
         <v>0</v>
       </c>
-      <c r="H5" s="148"/>
-      <c r="I5" s="148"/>
-      <c r="J5" s="148"/>
-      <c r="K5" s="148"/>
-      <c r="L5" s="148"/>
-      <c r="M5" s="149"/>
-      <c r="N5" s="150"/>
-      <c r="O5" s="150"/>
-      <c r="P5" s="150"/>
-      <c r="Q5" s="151"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="49"/>
+      <c r="N5" s="50"/>
+      <c r="O5" s="50"/>
+      <c r="P5" s="50"/>
+      <c r="Q5" s="51"/>
     </row>
     <row r="6" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="131"/>
-      <c r="B6" s="132"/>
-      <c r="C6" s="132"/>
-      <c r="D6" s="132"/>
-      <c r="E6" s="132"/>
-      <c r="F6" s="132"/>
-      <c r="G6" s="132"/>
-      <c r="H6" s="132"/>
-      <c r="I6" s="132"/>
-      <c r="J6" s="132"/>
-      <c r="K6" s="132"/>
-      <c r="L6" s="132"/>
-      <c r="M6" s="132"/>
-      <c r="N6" s="132"/>
-      <c r="O6" s="132"/>
-      <c r="P6" s="132"/>
-      <c r="Q6" s="133"/>
+      <c r="A6" s="42"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="43"/>
+      <c r="M6" s="43"/>
+      <c r="N6" s="43"/>
+      <c r="O6" s="43"/>
+      <c r="P6" s="43"/>
+      <c r="Q6" s="44"/>
     </row>
     <row r="7" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="78" t="s">
+      <c r="A7" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="79"/>
-      <c r="C7" s="79"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="79"/>
-      <c r="G7" s="79"/>
-      <c r="H7" s="79"/>
-      <c r="I7" s="79"/>
-      <c r="J7" s="79"/>
-      <c r="K7" s="79"/>
-      <c r="L7" s="79"/>
-      <c r="M7" s="79"/>
-      <c r="N7" s="79"/>
-      <c r="O7" s="79"/>
-      <c r="P7" s="79"/>
-      <c r="Q7" s="80"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="53"/>
+      <c r="M7" s="53"/>
+      <c r="N7" s="53"/>
+      <c r="O7" s="53"/>
+      <c r="P7" s="53"/>
+      <c r="Q7" s="54"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="81"/>
-      <c r="B8" s="82"/>
-      <c r="C8" s="82"/>
-      <c r="D8" s="87" t="s">
+      <c r="A8" s="55"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="91"/>
-      <c r="F8" s="91"/>
-      <c r="G8" s="88"/>
-      <c r="H8" s="87" t="s">
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="91"/>
-      <c r="J8" s="91"/>
-      <c r="K8" s="91"/>
-      <c r="L8" s="91"/>
-      <c r="M8" s="88"/>
-      <c r="N8" s="91" t="s">
+      <c r="I8" s="60"/>
+      <c r="J8" s="60"/>
+      <c r="K8" s="60"/>
+      <c r="L8" s="60"/>
+      <c r="M8" s="61"/>
+      <c r="N8" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="O8" s="91"/>
-      <c r="P8" s="91"/>
-      <c r="Q8" s="88"/>
+      <c r="O8" s="60"/>
+      <c r="P8" s="60"/>
+      <c r="Q8" s="61"/>
     </row>
     <row r="9" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="134"/>
-      <c r="B9" s="135"/>
-      <c r="C9" s="135"/>
-      <c r="D9" s="101"/>
-      <c r="E9" s="112"/>
-      <c r="F9" s="112"/>
-      <c r="G9" s="102"/>
-      <c r="H9" s="101"/>
-      <c r="I9" s="112"/>
-      <c r="J9" s="112"/>
-      <c r="K9" s="112"/>
-      <c r="L9" s="112"/>
-      <c r="M9" s="102"/>
-      <c r="N9" s="112"/>
-      <c r="O9" s="112"/>
-      <c r="P9" s="112"/>
-      <c r="Q9" s="102"/>
+      <c r="A9" s="57"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="62"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="64"/>
+      <c r="N9" s="63"/>
+      <c r="O9" s="63"/>
+      <c r="P9" s="63"/>
+      <c r="Q9" s="64"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="126"/>
-      <c r="B10" s="127"/>
-      <c r="C10" s="128"/>
-      <c r="D10" s="129" t="s">
+      <c r="A10" s="88"/>
+      <c r="B10" s="89"/>
+      <c r="C10" s="90"/>
+      <c r="D10" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="113"/>
-      <c r="F10" s="113" t="s">
+      <c r="E10" s="77"/>
+      <c r="F10" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="114"/>
-      <c r="H10" s="129" t="s">
+      <c r="G10" s="78"/>
+      <c r="H10" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="I10" s="113"/>
-      <c r="J10" s="113"/>
-      <c r="K10" s="113" t="s">
+      <c r="I10" s="77"/>
+      <c r="J10" s="77"/>
+      <c r="K10" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="L10" s="113"/>
-      <c r="M10" s="114"/>
-      <c r="N10" s="130" t="s">
+      <c r="L10" s="77"/>
+      <c r="M10" s="78"/>
+      <c r="N10" s="92" t="s">
         <v>36</v>
       </c>
-      <c r="O10" s="113"/>
-      <c r="P10" s="113" t="s">
+      <c r="O10" s="77"/>
+      <c r="P10" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="Q10" s="114"/>
+      <c r="Q10" s="78"/>
     </row>
     <row r="11" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="115"/>
-      <c r="B11" s="116"/>
-      <c r="C11" s="117"/>
+      <c r="A11" s="79"/>
+      <c r="B11" s="80"/>
+      <c r="C11" s="81"/>
       <c r="D11" s="7" t="s">
         <v>7</v>
       </c>
@@ -2005,30 +2013,30 @@
       </c>
     </row>
     <row r="12" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="118"/>
-      <c r="B12" s="119"/>
-      <c r="C12" s="119"/>
-      <c r="D12" s="119"/>
-      <c r="E12" s="119"/>
-      <c r="F12" s="119"/>
-      <c r="G12" s="119"/>
-      <c r="H12" s="119"/>
-      <c r="I12" s="119"/>
-      <c r="J12" s="119"/>
-      <c r="K12" s="119"/>
-      <c r="L12" s="119"/>
-      <c r="M12" s="119"/>
-      <c r="N12" s="119"/>
-      <c r="O12" s="119"/>
-      <c r="P12" s="119"/>
-      <c r="Q12" s="120"/>
+      <c r="A12" s="82"/>
+      <c r="B12" s="83"/>
+      <c r="C12" s="83"/>
+      <c r="D12" s="83"/>
+      <c r="E12" s="83"/>
+      <c r="F12" s="83"/>
+      <c r="G12" s="83"/>
+      <c r="H12" s="83"/>
+      <c r="I12" s="83"/>
+      <c r="J12" s="83"/>
+      <c r="K12" s="83"/>
+      <c r="L12" s="83"/>
+      <c r="M12" s="83"/>
+      <c r="N12" s="83"/>
+      <c r="O12" s="83"/>
+      <c r="P12" s="83"/>
+      <c r="Q12" s="84"/>
     </row>
     <row r="13" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="121" t="s">
+      <c r="A13" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="122"/>
-      <c r="C13" s="123"/>
+      <c r="B13" s="66"/>
+      <c r="C13" s="67"/>
       <c r="D13" s="20" t="str">
         <f t="array" ref="D13">IFERROR(INDEX(Spaces!$E:$E,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Acc.")*(Spaces!$D:$D="Standard"),0)),"")</f>
         <v/>
@@ -2077,11 +2085,11 @@
       </c>
     </row>
     <row r="14" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="121" t="s">
+      <c r="A14" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="122"/>
-      <c r="C14" s="123"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="67"/>
       <c r="D14" s="20" t="str">
         <f t="array" ref="D14">IFERROR(INDEX(Spaces!$E:$E,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Acc.")*(Spaces!$D:$D="Title I"),0)),"")</f>
         <v/>
@@ -2098,12 +2106,12 @@
         <f t="array" ref="G14">IFERROR(INDEX(Spaces!$E:$E,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Una")*(Spaces!$D:$D="Title I"),0)),"")</f>
         <v/>
       </c>
-      <c r="H14" s="64"/>
-      <c r="I14" s="124"/>
-      <c r="J14" s="124"/>
-      <c r="K14" s="124"/>
-      <c r="L14" s="124"/>
-      <c r="M14" s="125"/>
+      <c r="H14" s="85"/>
+      <c r="I14" s="86"/>
+      <c r="J14" s="86"/>
+      <c r="K14" s="86"/>
+      <c r="L14" s="86"/>
+      <c r="M14" s="87"/>
       <c r="N14" s="20" t="str">
         <f t="array" ref="N14">IFERROR(INDEX(Spaces!$E:$E,MATCH(1,(Spaces!$A:$A="School-age")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Acc.")*(Spaces!$D:$D="Title I"),0)),"")</f>
         <v/>
@@ -2122,860 +2130,912 @@
       </c>
     </row>
     <row r="15" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="121" t="s">
+      <c r="A15" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="122"/>
-      <c r="C15" s="123"/>
-      <c r="D15" s="152" t="str">
+      <c r="B15" s="66"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="27" t="str">
         <f t="array" ref="D15">IFERROR(INDEX(Spaces!$F:$F,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Acc."),0)),"")</f>
         <v/>
       </c>
-      <c r="E15" s="153" t="str">
+      <c r="E15" s="28" t="str">
         <f t="array" ref="E15">IFERROR(INDEX(Spaces!$F:$F,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Una"),0)),"")</f>
         <v/>
       </c>
-      <c r="F15" s="153" t="str">
+      <c r="F15" s="28" t="str">
         <f t="array" ref="F15">IFERROR(INDEX(Spaces!$F:$F,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Acc."),0)),"")</f>
         <v/>
       </c>
-      <c r="G15" s="154" t="str">
+      <c r="G15" s="29" t="str">
         <f t="array" ref="G15">IFERROR(INDEX(Spaces!$F:$F,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Una"),0)),"")</f>
         <v/>
       </c>
-      <c r="H15" s="152" t="str">
+      <c r="H15" s="27" t="str">
         <f t="array" ref="H15">IFERROR(INDEX(Spaces!$F:$F,MATCH(1,(Spaces!$A:$A="Preschool")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Acc."),0)),"")</f>
         <v/>
       </c>
-      <c r="I15" s="155"/>
-      <c r="J15" s="153" t="str">
+      <c r="I15" s="30"/>
+      <c r="J15" s="28" t="str">
         <f t="array" ref="J15">IFERROR(INDEX(Spaces!$F:$F,MATCH(1,(Spaces!$A:$A="Preschool")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Una"),0)),"")</f>
         <v/>
       </c>
-      <c r="K15" s="153" t="str">
+      <c r="K15" s="28" t="str">
         <f t="array" ref="K15">IFERROR(INDEX(Spaces!$F:$F,MATCH(1,(Spaces!$A:$A="Preschool")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Acc."),0)),"")</f>
         <v/>
       </c>
-      <c r="L15" s="155"/>
-      <c r="M15" s="154" t="str">
+      <c r="L15" s="30"/>
+      <c r="M15" s="29" t="str">
         <f t="array" ref="M15">IFERROR(INDEX(Spaces!$F:$F,MATCH(1,(Spaces!$A:$A="Preschool")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Una"),0)),"")</f>
         <v/>
       </c>
-      <c r="N15" s="156" t="str">
+      <c r="N15" s="31" t="str">
         <f t="array" ref="N15">IFERROR(INDEX(Spaces!$F:$F,MATCH(1,(Spaces!$A:$A="School-age")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Acc."),0)),"")</f>
         <v/>
       </c>
-      <c r="O15" s="153" t="str">
+      <c r="O15" s="28" t="str">
         <f t="array" ref="O15">IFERROR(INDEX(Spaces!$F:$F,MATCH(1,(Spaces!$A:$A="School-age")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Una"),0)),"")</f>
         <v/>
       </c>
-      <c r="P15" s="153" t="str">
+      <c r="P15" s="28" t="str">
         <f t="array" ref="P15">IFERROR(INDEX(Spaces!$F:$F,MATCH(1,(Spaces!$A:$A="School-age")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Acc."),0)),"")</f>
         <v/>
       </c>
-      <c r="Q15" s="154" t="str">
+      <c r="Q15" s="29" t="str">
         <f t="array" ref="Q15">IFERROR(INDEX(Spaces!$F:$F,MATCH(1,(Spaces!$A:$A="School-age")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Una"),0)),"")</f>
         <v/>
       </c>
     </row>
     <row r="16" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="121" t="s">
+      <c r="A16" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="122"/>
-      <c r="C16" s="123"/>
-      <c r="D16" s="152" t="str">
+      <c r="B16" s="66"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="27" t="str">
         <f t="array" ref="D16">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Acc.")*(Spaces!$D:$D="Standard"),0)),"")</f>
         <v/>
       </c>
-      <c r="E16" s="153" t="str">
+      <c r="E16" s="28" t="str">
         <f t="array" ref="E16">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Una")*(Spaces!$D:$D="Standard"),0)),"")</f>
         <v/>
       </c>
-      <c r="F16" s="153" t="str">
+      <c r="F16" s="28" t="str">
         <f t="array" ref="F16">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Acc.")*(Spaces!$D:$D="Standard"),0)),"")</f>
         <v/>
       </c>
-      <c r="G16" s="154" t="str">
+      <c r="G16" s="29" t="str">
         <f t="array" ref="G16">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Una")*(Spaces!$D:$D="Standard"),0)),"")</f>
         <v/>
       </c>
-      <c r="H16" s="152" t="str">
+      <c r="H16" s="27" t="str">
         <f t="array" ref="H16">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="Preschool")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Acc."),0)),"")</f>
         <v/>
       </c>
-      <c r="I16" s="155"/>
-      <c r="J16" s="153" t="str">
+      <c r="I16" s="30"/>
+      <c r="J16" s="28" t="str">
         <f t="array" ref="J16">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="Preschool")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Una"),0)),"")</f>
         <v/>
       </c>
-      <c r="K16" s="153" t="str">
+      <c r="K16" s="28" t="str">
         <f t="array" ref="K16">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="Preschool")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Acc."),0)),"")</f>
         <v/>
       </c>
-      <c r="L16" s="155"/>
-      <c r="M16" s="154" t="str">
+      <c r="L16" s="30"/>
+      <c r="M16" s="29" t="str">
         <f t="array" ref="M16">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="Preschool")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Una"),0)),"")</f>
         <v/>
       </c>
-      <c r="N16" s="156" t="str">
+      <c r="N16" s="31" t="str">
         <f t="array" ref="N16">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="School-age")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Acc.")*(Spaces!$D:$D="Standard"),0)),"")</f>
         <v/>
       </c>
-      <c r="O16" s="153" t="str">
+      <c r="O16" s="28" t="str">
         <f t="array" ref="O16">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="School-age")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Una")*(Spaces!$D:$D="Standard"),0)),"")</f>
         <v/>
       </c>
-      <c r="P16" s="153" t="str">
+      <c r="P16" s="28" t="str">
         <f t="array" ref="P16">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="School-age")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Acc.")*(Spaces!$D:$D="Standard"),0)),"")</f>
         <v/>
       </c>
-      <c r="Q16" s="154" t="str">
+      <c r="Q16" s="29" t="str">
         <f t="array" ref="Q16">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="School-age")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Una")*(Spaces!$D:$D="Standard"),0)),"")</f>
         <v/>
       </c>
     </row>
     <row r="17" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="136" t="s">
+      <c r="A17" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="137"/>
-      <c r="C17" s="138"/>
-      <c r="D17" s="157" t="str">
+      <c r="B17" s="69"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="32" t="str">
         <f t="array" ref="D17">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Acc.")*(Spaces!$D:$D="Title I"),0)),"")</f>
         <v/>
       </c>
-      <c r="E17" s="158" t="str">
+      <c r="E17" s="33" t="str">
         <f t="array" ref="E17">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Una")*(Spaces!$D:$D="Title I"),0)),"")</f>
         <v/>
       </c>
-      <c r="F17" s="158" t="str">
+      <c r="F17" s="33" t="str">
         <f t="array" ref="F17">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Acc.")*(Spaces!$D:$D="Title I"),0)),"")</f>
         <v/>
       </c>
-      <c r="G17" s="159" t="str">
+      <c r="G17" s="34" t="str">
         <f t="array" ref="G17">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Una")*(Spaces!$D:$D="Title I"),0)),"")</f>
         <v/>
       </c>
-      <c r="H17" s="160"/>
-      <c r="I17" s="161"/>
-      <c r="J17" s="161"/>
-      <c r="K17" s="161"/>
-      <c r="L17" s="161"/>
-      <c r="M17" s="162"/>
-      <c r="N17" s="163" t="str">
+      <c r="H17" s="71"/>
+      <c r="I17" s="72"/>
+      <c r="J17" s="72"/>
+      <c r="K17" s="72"/>
+      <c r="L17" s="72"/>
+      <c r="M17" s="73"/>
+      <c r="N17" s="35" t="str">
         <f t="array" ref="N17">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="School-age")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Acc.")*(Spaces!$D:$D="Title I"),0)),"")</f>
         <v/>
       </c>
-      <c r="O17" s="158" t="str">
+      <c r="O17" s="33" t="str">
         <f t="array" ref="O17">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="School-age")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Una")*(Spaces!$D:$D="Title I"),0)),"")</f>
         <v/>
       </c>
-      <c r="P17" s="158" t="str">
+      <c r="P17" s="33" t="str">
         <f t="array" ref="P17">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="School-age")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Acc.")*(Spaces!$D:$D="Title I"),0)),"")</f>
         <v/>
       </c>
-      <c r="Q17" s="159" t="str">
+      <c r="Q17" s="34" t="str">
         <f t="array" ref="Q17">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="School-age")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Una")*(Spaces!$D:$D="Title I"),0)),"")</f>
         <v/>
       </c>
     </row>
     <row r="18" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="75"/>
-      <c r="B18" s="76"/>
-      <c r="C18" s="76"/>
-      <c r="D18" s="76"/>
-      <c r="E18" s="76"/>
-      <c r="F18" s="76"/>
-      <c r="G18" s="76"/>
-      <c r="H18" s="76"/>
-      <c r="I18" s="76"/>
-      <c r="J18" s="76"/>
-      <c r="K18" s="76"/>
-      <c r="L18" s="76"/>
-      <c r="M18" s="76"/>
-      <c r="N18" s="76"/>
-      <c r="O18" s="76"/>
-      <c r="P18" s="76"/>
-      <c r="Q18" s="77"/>
+      <c r="A18" s="74"/>
+      <c r="B18" s="75"/>
+      <c r="C18" s="75"/>
+      <c r="D18" s="75"/>
+      <c r="E18" s="75"/>
+      <c r="F18" s="75"/>
+      <c r="G18" s="75"/>
+      <c r="H18" s="75"/>
+      <c r="I18" s="75"/>
+      <c r="J18" s="75"/>
+      <c r="K18" s="75"/>
+      <c r="L18" s="75"/>
+      <c r="M18" s="75"/>
+      <c r="N18" s="75"/>
+      <c r="O18" s="75"/>
+      <c r="P18" s="75"/>
+      <c r="Q18" s="76"/>
     </row>
     <row r="19" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="78" t="s">
+      <c r="A19" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="79"/>
-      <c r="C19" s="79"/>
-      <c r="D19" s="79"/>
-      <c r="E19" s="79"/>
-      <c r="F19" s="79"/>
-      <c r="G19" s="79"/>
-      <c r="H19" s="79"/>
-      <c r="I19" s="79"/>
-      <c r="J19" s="79"/>
-      <c r="K19" s="79"/>
-      <c r="L19" s="79"/>
-      <c r="M19" s="79"/>
-      <c r="N19" s="79"/>
-      <c r="O19" s="80"/>
+      <c r="B19" s="53"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="53"/>
+      <c r="G19" s="53"/>
+      <c r="H19" s="53"/>
+      <c r="I19" s="53"/>
+      <c r="J19" s="53"/>
+      <c r="K19" s="53"/>
+      <c r="L19" s="53"/>
+      <c r="M19" s="53"/>
+      <c r="N19" s="53"/>
+      <c r="O19" s="54"/>
       <c r="P19" s="3"/>
       <c r="Q19" s="4"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A20" s="81"/>
-      <c r="B20" s="82"/>
-      <c r="C20" s="83"/>
-      <c r="D20" s="87" t="s">
+      <c r="A20" s="55"/>
+      <c r="B20" s="56"/>
+      <c r="C20" s="108"/>
+      <c r="D20" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="88"/>
-      <c r="F20" s="91" t="s">
+      <c r="E20" s="61"/>
+      <c r="F20" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="88"/>
-      <c r="H20" s="87" t="s">
+      <c r="G20" s="61"/>
+      <c r="H20" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="I20" s="91"/>
-      <c r="J20" s="87" t="s">
+      <c r="I20" s="60"/>
+      <c r="J20" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="K20" s="88"/>
-      <c r="L20" s="91" t="s">
+      <c r="K20" s="61"/>
+      <c r="L20" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="M20" s="88"/>
-      <c r="N20" s="87" t="s">
+      <c r="M20" s="61"/>
+      <c r="N20" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="O20" s="88"/>
+      <c r="O20" s="61"/>
       <c r="P20" s="3"/>
       <c r="Q20" s="4"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A21" s="84"/>
-      <c r="B21" s="85"/>
-      <c r="C21" s="86"/>
-      <c r="D21" s="101"/>
-      <c r="E21" s="102"/>
-      <c r="F21" s="112"/>
-      <c r="G21" s="102"/>
-      <c r="H21" s="101"/>
-      <c r="I21" s="112"/>
-      <c r="J21" s="101"/>
-      <c r="K21" s="102"/>
-      <c r="L21" s="112"/>
-      <c r="M21" s="102"/>
-      <c r="N21" s="101"/>
-      <c r="O21" s="102"/>
+      <c r="A21" s="109"/>
+      <c r="B21" s="110"/>
+      <c r="C21" s="111"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="63"/>
+      <c r="G21" s="64"/>
+      <c r="H21" s="62"/>
+      <c r="I21" s="63"/>
+      <c r="J21" s="62"/>
+      <c r="K21" s="64"/>
+      <c r="L21" s="63"/>
+      <c r="M21" s="64"/>
+      <c r="N21" s="62"/>
+      <c r="O21" s="64"/>
       <c r="P21" s="3"/>
       <c r="Q21" s="4"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A22" s="103"/>
-      <c r="B22" s="104"/>
-      <c r="C22" s="105"/>
-      <c r="D22" s="96">
+      <c r="A22" s="93"/>
+      <c r="B22" s="94"/>
+      <c r="C22" s="95"/>
+      <c r="D22" s="102">
         <v>1</v>
       </c>
-      <c r="E22" s="97"/>
-      <c r="F22" s="93">
+      <c r="E22" s="103"/>
+      <c r="F22" s="104">
         <v>24280</v>
       </c>
-      <c r="G22" s="94"/>
-      <c r="H22" s="98">
+      <c r="G22" s="105"/>
+      <c r="H22" s="106">
         <f>'Family Income Groupings'!C2</f>
         <v>0</v>
       </c>
-      <c r="I22" s="98"/>
-      <c r="J22" s="96">
+      <c r="I22" s="106"/>
+      <c r="J22" s="102">
         <v>7</v>
       </c>
-      <c r="K22" s="97"/>
-      <c r="L22" s="93">
+      <c r="K22" s="103"/>
+      <c r="L22" s="104">
         <v>76120</v>
       </c>
-      <c r="M22" s="94"/>
-      <c r="N22" s="95">
+      <c r="M22" s="105"/>
+      <c r="N22" s="107">
         <f>'Family Income Groupings'!C8</f>
         <v>0</v>
       </c>
-      <c r="O22" s="95"/>
+      <c r="O22" s="107"/>
       <c r="P22" s="3"/>
       <c r="Q22" s="4"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A23" s="106"/>
-      <c r="B23" s="107"/>
-      <c r="C23" s="108"/>
-      <c r="D23" s="96">
+      <c r="A23" s="96"/>
+      <c r="B23" s="97"/>
+      <c r="C23" s="98"/>
+      <c r="D23" s="102">
         <v>2</v>
       </c>
-      <c r="E23" s="97"/>
-      <c r="F23" s="93">
+      <c r="E23" s="103"/>
+      <c r="F23" s="104">
         <v>32920</v>
       </c>
-      <c r="G23" s="94"/>
-      <c r="H23" s="98">
+      <c r="G23" s="105"/>
+      <c r="H23" s="106">
         <f>'Family Income Groupings'!C3</f>
         <v>0</v>
       </c>
-      <c r="I23" s="98"/>
-      <c r="J23" s="96">
+      <c r="I23" s="106"/>
+      <c r="J23" s="102">
         <v>8</v>
       </c>
-      <c r="K23" s="97"/>
-      <c r="L23" s="93">
+      <c r="K23" s="103"/>
+      <c r="L23" s="104">
         <v>84760</v>
       </c>
-      <c r="M23" s="94"/>
-      <c r="N23" s="95">
+      <c r="M23" s="105"/>
+      <c r="N23" s="107">
         <f>'Family Income Groupings'!C9</f>
         <v>0</v>
       </c>
-      <c r="O23" s="95"/>
+      <c r="O23" s="107"/>
       <c r="P23" s="3"/>
       <c r="Q23" s="4"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A24" s="106"/>
-      <c r="B24" s="107"/>
-      <c r="C24" s="108"/>
-      <c r="D24" s="96">
+      <c r="A24" s="96"/>
+      <c r="B24" s="97"/>
+      <c r="C24" s="98"/>
+      <c r="D24" s="102">
         <v>3</v>
       </c>
-      <c r="E24" s="97"/>
-      <c r="F24" s="93">
+      <c r="E24" s="103"/>
+      <c r="F24" s="104">
         <v>41560</v>
       </c>
-      <c r="G24" s="94"/>
-      <c r="H24" s="98">
+      <c r="G24" s="105"/>
+      <c r="H24" s="106">
         <f>'Family Income Groupings'!C4</f>
         <v>0</v>
       </c>
-      <c r="I24" s="98"/>
-      <c r="J24" s="96">
+      <c r="I24" s="106"/>
+      <c r="J24" s="102">
         <v>9</v>
       </c>
-      <c r="K24" s="97"/>
-      <c r="L24" s="93">
+      <c r="K24" s="103"/>
+      <c r="L24" s="104">
         <v>93400</v>
       </c>
-      <c r="M24" s="94"/>
-      <c r="N24" s="95">
+      <c r="M24" s="105"/>
+      <c r="N24" s="107">
         <f>'Family Income Groupings'!C10</f>
         <v>0</v>
       </c>
-      <c r="O24" s="95"/>
+      <c r="O24" s="107"/>
       <c r="P24" s="3"/>
       <c r="Q24" s="4"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A25" s="106"/>
-      <c r="B25" s="107"/>
-      <c r="C25" s="108"/>
-      <c r="D25" s="96">
+      <c r="A25" s="96"/>
+      <c r="B25" s="97"/>
+      <c r="C25" s="98"/>
+      <c r="D25" s="102">
         <v>4</v>
       </c>
-      <c r="E25" s="97"/>
-      <c r="F25" s="93">
+      <c r="E25" s="103"/>
+      <c r="F25" s="104">
         <v>50200</v>
       </c>
-      <c r="G25" s="94"/>
-      <c r="H25" s="98">
+      <c r="G25" s="105"/>
+      <c r="H25" s="106">
         <f>'Family Income Groupings'!C5</f>
         <v>0</v>
       </c>
-      <c r="I25" s="98"/>
-      <c r="J25" s="96">
+      <c r="I25" s="106"/>
+      <c r="J25" s="102">
         <v>10</v>
       </c>
-      <c r="K25" s="97"/>
-      <c r="L25" s="93">
+      <c r="K25" s="103"/>
+      <c r="L25" s="104">
         <v>102040</v>
       </c>
-      <c r="M25" s="94"/>
-      <c r="N25" s="95">
+      <c r="M25" s="105"/>
+      <c r="N25" s="107">
         <f>'Family Income Groupings'!C11</f>
         <v>0</v>
       </c>
-      <c r="O25" s="95"/>
+      <c r="O25" s="107"/>
       <c r="P25" s="3"/>
       <c r="Q25" s="4"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A26" s="106"/>
-      <c r="B26" s="107"/>
-      <c r="C26" s="108"/>
-      <c r="D26" s="96">
+      <c r="A26" s="96"/>
+      <c r="B26" s="97"/>
+      <c r="C26" s="98"/>
+      <c r="D26" s="102">
         <v>5</v>
       </c>
-      <c r="E26" s="97"/>
-      <c r="F26" s="93">
+      <c r="E26" s="103"/>
+      <c r="F26" s="104">
         <v>58840</v>
       </c>
-      <c r="G26" s="94"/>
-      <c r="H26" s="98">
+      <c r="G26" s="105"/>
+      <c r="H26" s="106">
         <f>'Family Income Groupings'!C6</f>
         <v>0</v>
       </c>
-      <c r="I26" s="98"/>
-      <c r="J26" s="96">
+      <c r="I26" s="106"/>
+      <c r="J26" s="102">
         <v>11</v>
       </c>
-      <c r="K26" s="97"/>
-      <c r="L26" s="93">
+      <c r="K26" s="103"/>
+      <c r="L26" s="104">
         <v>110680</v>
       </c>
-      <c r="M26" s="94"/>
-      <c r="N26" s="95">
+      <c r="M26" s="105"/>
+      <c r="N26" s="107">
         <f>'Family Income Groupings'!C12</f>
         <v>0</v>
       </c>
-      <c r="O26" s="95"/>
+      <c r="O26" s="107"/>
       <c r="P26" s="3"/>
       <c r="Q26" s="4"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A27" s="109"/>
-      <c r="B27" s="110"/>
-      <c r="C27" s="111"/>
-      <c r="D27" s="99">
+      <c r="A27" s="99"/>
+      <c r="B27" s="100"/>
+      <c r="C27" s="101"/>
+      <c r="D27" s="112">
         <v>6</v>
       </c>
-      <c r="E27" s="99"/>
-      <c r="F27" s="100">
+      <c r="E27" s="112"/>
+      <c r="F27" s="113">
         <v>67480</v>
       </c>
-      <c r="G27" s="100"/>
-      <c r="H27" s="98">
+      <c r="G27" s="113"/>
+      <c r="H27" s="106">
         <f>'Family Income Groupings'!C7</f>
         <v>0</v>
       </c>
-      <c r="I27" s="98"/>
-      <c r="J27" s="99">
+      <c r="I27" s="106"/>
+      <c r="J27" s="112">
         <v>12</v>
       </c>
-      <c r="K27" s="99"/>
-      <c r="L27" s="100">
+      <c r="K27" s="112"/>
+      <c r="L27" s="113">
         <v>119320</v>
       </c>
-      <c r="M27" s="100"/>
-      <c r="N27" s="95">
+      <c r="M27" s="113"/>
+      <c r="N27" s="107">
         <f>'Family Income Groupings'!C13</f>
         <v>0</v>
       </c>
-      <c r="O27" s="95"/>
+      <c r="O27" s="107"/>
       <c r="P27" s="3"/>
       <c r="Q27" s="4"/>
     </row>
     <row r="28" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="75"/>
-      <c r="B28" s="76"/>
-      <c r="C28" s="76"/>
-      <c r="D28" s="76"/>
-      <c r="E28" s="76"/>
-      <c r="F28" s="76"/>
-      <c r="G28" s="76"/>
-      <c r="H28" s="76"/>
-      <c r="I28" s="76"/>
-      <c r="J28" s="76"/>
-      <c r="K28" s="76"/>
-      <c r="L28" s="76"/>
-      <c r="M28" s="76"/>
-      <c r="N28" s="76"/>
-      <c r="O28" s="76"/>
-      <c r="P28" s="76"/>
-      <c r="Q28" s="77"/>
+      <c r="A28" s="74"/>
+      <c r="B28" s="75"/>
+      <c r="C28" s="75"/>
+      <c r="D28" s="75"/>
+      <c r="E28" s="75"/>
+      <c r="F28" s="75"/>
+      <c r="G28" s="75"/>
+      <c r="H28" s="75"/>
+      <c r="I28" s="75"/>
+      <c r="J28" s="75"/>
+      <c r="K28" s="75"/>
+      <c r="L28" s="75"/>
+      <c r="M28" s="75"/>
+      <c r="N28" s="75"/>
+      <c r="O28" s="75"/>
+      <c r="P28" s="75"/>
+      <c r="Q28" s="76"/>
     </row>
     <row r="29" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="78" t="s">
+      <c r="A29" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="79"/>
-      <c r="C29" s="79"/>
-      <c r="D29" s="79"/>
-      <c r="E29" s="79"/>
-      <c r="F29" s="79"/>
-      <c r="G29" s="79"/>
-      <c r="H29" s="79"/>
-      <c r="I29" s="79"/>
-      <c r="J29" s="79"/>
-      <c r="K29" s="79"/>
-      <c r="L29" s="79"/>
-      <c r="M29" s="79"/>
-      <c r="N29" s="79"/>
-      <c r="O29" s="80"/>
+      <c r="B29" s="53"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="53"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="53"/>
+      <c r="J29" s="53"/>
+      <c r="K29" s="53"/>
+      <c r="L29" s="53"/>
+      <c r="M29" s="53"/>
+      <c r="N29" s="53"/>
+      <c r="O29" s="54"/>
       <c r="P29" s="5"/>
       <c r="Q29" s="8"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A30" s="81"/>
-      <c r="B30" s="82"/>
-      <c r="C30" s="83"/>
-      <c r="D30" s="87"/>
-      <c r="E30" s="88"/>
-      <c r="F30" s="91" t="s">
+      <c r="A30" s="55"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="108"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="61"/>
+      <c r="F30" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="G30" s="88"/>
-      <c r="H30" s="87" t="s">
+      <c r="G30" s="61"/>
+      <c r="H30" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="I30" s="91"/>
-      <c r="J30" s="87" t="s">
+      <c r="I30" s="60"/>
+      <c r="J30" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="K30" s="88"/>
-      <c r="L30" s="91" t="s">
+      <c r="K30" s="61"/>
+      <c r="L30" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="M30" s="88"/>
-      <c r="N30" s="87" t="s">
+      <c r="M30" s="61"/>
+      <c r="N30" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="O30" s="88"/>
+      <c r="O30" s="61"/>
       <c r="P30" s="3"/>
       <c r="Q30" s="4"/>
     </row>
     <row r="31" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="84"/>
-      <c r="B31" s="85"/>
-      <c r="C31" s="86"/>
-      <c r="D31" s="89"/>
-      <c r="E31" s="90"/>
-      <c r="F31" s="92"/>
-      <c r="G31" s="90"/>
-      <c r="H31" s="89"/>
-      <c r="I31" s="92"/>
-      <c r="J31" s="89"/>
-      <c r="K31" s="90"/>
-      <c r="L31" s="92"/>
-      <c r="M31" s="90"/>
-      <c r="N31" s="89"/>
-      <c r="O31" s="90"/>
+      <c r="A31" s="109"/>
+      <c r="B31" s="110"/>
+      <c r="C31" s="111"/>
+      <c r="D31" s="114"/>
+      <c r="E31" s="115"/>
+      <c r="F31" s="116"/>
+      <c r="G31" s="115"/>
+      <c r="H31" s="114"/>
+      <c r="I31" s="116"/>
+      <c r="J31" s="114"/>
+      <c r="K31" s="115"/>
+      <c r="L31" s="116"/>
+      <c r="M31" s="115"/>
+      <c r="N31" s="114"/>
+      <c r="O31" s="115"/>
       <c r="P31" s="3"/>
       <c r="Q31" s="4"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A32" s="69" t="s">
+      <c r="A32" s="126" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="70"/>
-      <c r="C32" s="71"/>
-      <c r="D32" s="57"/>
-      <c r="E32" s="58"/>
-      <c r="F32" s="62">
+      <c r="B32" s="127"/>
+      <c r="C32" s="128"/>
+      <c r="D32" s="117"/>
+      <c r="E32" s="118"/>
+      <c r="F32" s="129">
         <f>IFERROR((G5*D13)*D16,0)+IFERROR((G5*D14)*D17,0)+IFERROR((G5*E13)*E16,0)+IFERROR((G5*E14)*E17,0)</f>
         <v>0</v>
       </c>
-      <c r="G32" s="63"/>
-      <c r="H32" s="72"/>
-      <c r="I32" s="73"/>
-      <c r="J32" s="74"/>
-      <c r="K32" s="73"/>
-      <c r="L32" s="74"/>
-      <c r="M32" s="73"/>
-      <c r="N32" s="57"/>
-      <c r="O32" s="58"/>
+      <c r="G32" s="130"/>
+      <c r="H32" s="131"/>
+      <c r="I32" s="132"/>
+      <c r="J32" s="133"/>
+      <c r="K32" s="132"/>
+      <c r="L32" s="133"/>
+      <c r="M32" s="132"/>
+      <c r="N32" s="117"/>
+      <c r="O32" s="118"/>
       <c r="P32" s="9"/>
       <c r="Q32" s="10"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A33" s="59" t="s">
+      <c r="A33" s="119" t="s">
         <v>25</v>
       </c>
-      <c r="B33" s="60"/>
-      <c r="C33" s="61"/>
-      <c r="D33" s="57"/>
-      <c r="E33" s="58"/>
-      <c r="F33" s="67">
+      <c r="B33" s="120"/>
+      <c r="C33" s="121"/>
+      <c r="D33" s="117"/>
+      <c r="E33" s="118"/>
+      <c r="F33" s="122">
         <f>IFERROR((G5*F13)*F16,0)+IFERROR((G5*F14)*F17,0)+IFERROR((G5*G13)*G16,0)+IFERROR((G5*G14)*G17,0)</f>
         <v>0</v>
       </c>
-      <c r="G33" s="68"/>
-      <c r="H33" s="64"/>
-      <c r="I33" s="65"/>
-      <c r="J33" s="66"/>
-      <c r="K33" s="65"/>
-      <c r="L33" s="66"/>
-      <c r="M33" s="65"/>
-      <c r="N33" s="57"/>
-      <c r="O33" s="58"/>
+      <c r="G33" s="123"/>
+      <c r="H33" s="85"/>
+      <c r="I33" s="124"/>
+      <c r="J33" s="125"/>
+      <c r="K33" s="124"/>
+      <c r="L33" s="125"/>
+      <c r="M33" s="124"/>
+      <c r="N33" s="117"/>
+      <c r="O33" s="118"/>
       <c r="P33" s="11"/>
       <c r="Q33" s="12"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A34" s="59" t="s">
+      <c r="A34" s="119" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="60"/>
-      <c r="C34" s="61"/>
-      <c r="D34" s="57"/>
-      <c r="E34" s="58"/>
-      <c r="F34" s="62">
+      <c r="B34" s="120"/>
+      <c r="C34" s="121"/>
+      <c r="D34" s="117"/>
+      <c r="E34" s="118"/>
+      <c r="F34" s="129">
         <f>IFERROR((G5*H13)*H16,0)+IFERROR((G5*I13)*I16,0)+IFERROR((G5*J13)*J16,0)</f>
         <v>0</v>
       </c>
-      <c r="G34" s="63"/>
-      <c r="H34" s="64"/>
-      <c r="I34" s="65"/>
-      <c r="J34" s="66"/>
-      <c r="K34" s="65"/>
-      <c r="L34" s="66"/>
-      <c r="M34" s="65"/>
-      <c r="N34" s="57"/>
-      <c r="O34" s="58"/>
+      <c r="G34" s="130"/>
+      <c r="H34" s="85"/>
+      <c r="I34" s="124"/>
+      <c r="J34" s="125"/>
+      <c r="K34" s="124"/>
+      <c r="L34" s="125"/>
+      <c r="M34" s="124"/>
+      <c r="N34" s="117"/>
+      <c r="O34" s="118"/>
       <c r="P34" s="11"/>
       <c r="Q34" s="12"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A35" s="59" t="s">
+      <c r="A35" s="119" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="60"/>
-      <c r="C35" s="61"/>
-      <c r="D35" s="57"/>
-      <c r="E35" s="58"/>
-      <c r="F35" s="62">
+      <c r="B35" s="120"/>
+      <c r="C35" s="121"/>
+      <c r="D35" s="117"/>
+      <c r="E35" s="118"/>
+      <c r="F35" s="129">
         <f>IFERROR((G5*K13)*K17,0)+IFERROR((G5*L13)*L17,0)+IFERROR((G5*M13)*M17,0)</f>
         <v>0</v>
       </c>
-      <c r="G35" s="63"/>
-      <c r="H35" s="64"/>
-      <c r="I35" s="65"/>
-      <c r="J35" s="66"/>
-      <c r="K35" s="65"/>
-      <c r="L35" s="66"/>
-      <c r="M35" s="65"/>
-      <c r="N35" s="57"/>
-      <c r="O35" s="58"/>
+      <c r="G35" s="130"/>
+      <c r="H35" s="85"/>
+      <c r="I35" s="124"/>
+      <c r="J35" s="125"/>
+      <c r="K35" s="124"/>
+      <c r="L35" s="125"/>
+      <c r="M35" s="124"/>
+      <c r="N35" s="117"/>
+      <c r="O35" s="118"/>
       <c r="P35" s="11"/>
       <c r="Q35" s="12"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A36" s="59" t="s">
+      <c r="A36" s="119" t="s">
         <v>28</v>
       </c>
-      <c r="B36" s="60"/>
-      <c r="C36" s="61"/>
-      <c r="D36" s="57"/>
-      <c r="E36" s="58"/>
-      <c r="F36" s="62">
+      <c r="B36" s="120"/>
+      <c r="C36" s="121"/>
+      <c r="D36" s="117"/>
+      <c r="E36" s="118"/>
+      <c r="F36" s="129">
         <f>IFERROR((G5*N13)*N16,0)+IFERROR((G5*N14)*N17,0)+IFERROR((G5*O13)*O16,0)+IFERROR((G5*O14)*O17,0)</f>
         <v>0</v>
       </c>
-      <c r="G36" s="63"/>
-      <c r="H36" s="64"/>
-      <c r="I36" s="65"/>
-      <c r="J36" s="66"/>
-      <c r="K36" s="65"/>
-      <c r="L36" s="66"/>
-      <c r="M36" s="65"/>
-      <c r="N36" s="57"/>
-      <c r="O36" s="58"/>
+      <c r="G36" s="130"/>
+      <c r="H36" s="85"/>
+      <c r="I36" s="124"/>
+      <c r="J36" s="125"/>
+      <c r="K36" s="124"/>
+      <c r="L36" s="125"/>
+      <c r="M36" s="124"/>
+      <c r="N36" s="117"/>
+      <c r="O36" s="118"/>
       <c r="P36" s="11"/>
       <c r="Q36" s="12"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A37" s="59" t="s">
+      <c r="A37" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="B37" s="60"/>
-      <c r="C37" s="61"/>
-      <c r="D37" s="57"/>
-      <c r="E37" s="58"/>
-      <c r="F37" s="62">
+      <c r="B37" s="120"/>
+      <c r="C37" s="121"/>
+      <c r="D37" s="117"/>
+      <c r="E37" s="118"/>
+      <c r="F37" s="129">
         <f>IFERROR((G5*P13)*P16,0)+IFERROR((G5*P14)*P17,0)+IFERROR((G5*Q13)*Q16,0)+IFERROR((G5*Q14)*Q17,0)</f>
         <v>0</v>
       </c>
-      <c r="G37" s="63"/>
-      <c r="H37" s="64"/>
-      <c r="I37" s="65"/>
-      <c r="J37" s="66"/>
-      <c r="K37" s="65"/>
-      <c r="L37" s="66"/>
-      <c r="M37" s="65"/>
-      <c r="N37" s="57"/>
-      <c r="O37" s="58"/>
+      <c r="G37" s="130"/>
+      <c r="H37" s="85"/>
+      <c r="I37" s="124"/>
+      <c r="J37" s="125"/>
+      <c r="K37" s="124"/>
+      <c r="L37" s="125"/>
+      <c r="M37" s="124"/>
+      <c r="N37" s="117"/>
+      <c r="O37" s="118"/>
       <c r="P37" s="11"/>
       <c r="Q37" s="12"/>
     </row>
     <row r="38" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="45" t="s">
+      <c r="A38" s="152" t="s">
         <v>30</v>
       </c>
-      <c r="B38" s="46"/>
-      <c r="C38" s="47"/>
-      <c r="D38" s="48"/>
-      <c r="E38" s="49"/>
-      <c r="F38" s="50">
+      <c r="B38" s="153"/>
+      <c r="C38" s="154"/>
+      <c r="D38" s="155"/>
+      <c r="E38" s="156"/>
+      <c r="F38" s="157">
         <f>SUM(F32:G37)</f>
         <v>0</v>
       </c>
-      <c r="G38" s="51"/>
-      <c r="H38" s="52">
+      <c r="G38" s="158"/>
+      <c r="H38" s="159">
         <f>'Other Details'!D2</f>
         <v>0</v>
       </c>
-      <c r="I38" s="53"/>
-      <c r="J38" s="54">
+      <c r="I38" s="160"/>
+      <c r="J38" s="161">
         <f>'Other Details'!E2</f>
         <v>0</v>
       </c>
-      <c r="K38" s="55"/>
-      <c r="L38" s="56">
+      <c r="K38" s="162"/>
+      <c r="L38" s="163">
         <f>'Other Details'!F2</f>
         <v>0</v>
       </c>
-      <c r="M38" s="53"/>
-      <c r="N38" s="33">
+      <c r="M38" s="160"/>
+      <c r="N38" s="140">
         <f t="shared" ref="N38" si="0">SUM(F38,H38,L38)</f>
         <v>0</v>
       </c>
-      <c r="O38" s="34"/>
+      <c r="O38" s="141"/>
       <c r="P38" s="11"/>
       <c r="Q38" s="12"/>
     </row>
     <row r="39" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="35"/>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="36"/>
-      <c r="I39" s="36"/>
-      <c r="J39" s="36"/>
-      <c r="K39" s="36"/>
-      <c r="L39" s="36"/>
-      <c r="M39" s="36"/>
+      <c r="A39" s="142"/>
+      <c r="B39" s="143"/>
+      <c r="C39" s="143"/>
+      <c r="D39" s="143"/>
+      <c r="E39" s="143"/>
+      <c r="F39" s="143"/>
+      <c r="G39" s="143"/>
+      <c r="H39" s="143"/>
+      <c r="I39" s="143"/>
+      <c r="J39" s="143"/>
+      <c r="K39" s="143"/>
+      <c r="L39" s="143"/>
+      <c r="M39" s="143"/>
       <c r="N39" s="5"/>
       <c r="O39" s="5"/>
       <c r="P39" s="5"/>
       <c r="Q39" s="8"/>
     </row>
     <row r="40" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="37" t="s">
+      <c r="A40" s="144" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="38"/>
-      <c r="C40" s="38"/>
-      <c r="D40" s="38"/>
-      <c r="E40" s="38"/>
-      <c r="F40" s="38"/>
-      <c r="G40" s="38"/>
-      <c r="H40" s="38"/>
-      <c r="I40" s="38"/>
-      <c r="J40" s="38"/>
-      <c r="K40" s="38"/>
-      <c r="L40" s="38"/>
-      <c r="M40" s="39"/>
+      <c r="B40" s="145"/>
+      <c r="C40" s="145"/>
+      <c r="D40" s="145"/>
+      <c r="E40" s="145"/>
+      <c r="F40" s="145"/>
+      <c r="G40" s="145"/>
+      <c r="H40" s="145"/>
+      <c r="I40" s="145"/>
+      <c r="J40" s="145"/>
+      <c r="K40" s="145"/>
+      <c r="L40" s="145"/>
+      <c r="M40" s="146"/>
       <c r="Q40" s="2"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A41" s="40" t="s">
+      <c r="A41" s="147" t="s">
         <v>32</v>
       </c>
-      <c r="B41" s="41"/>
-      <c r="C41" s="42" t="s">
+      <c r="B41" s="148"/>
+      <c r="C41" s="149" t="s">
         <v>35</v>
       </c>
-      <c r="D41" s="43"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="43"/>
-      <c r="G41" s="43"/>
-      <c r="H41" s="43"/>
-      <c r="I41" s="43"/>
-      <c r="J41" s="43"/>
-      <c r="K41" s="43"/>
-      <c r="L41" s="43"/>
-      <c r="M41" s="44"/>
+      <c r="D41" s="150"/>
+      <c r="E41" s="150"/>
+      <c r="F41" s="150"/>
+      <c r="G41" s="150"/>
+      <c r="H41" s="150"/>
+      <c r="I41" s="150"/>
+      <c r="J41" s="150"/>
+      <c r="K41" s="150"/>
+      <c r="L41" s="150"/>
+      <c r="M41" s="151"/>
       <c r="N41" s="23"/>
       <c r="O41" s="23"/>
       <c r="P41" s="23"/>
       <c r="Q41" s="24"/>
     </row>
     <row r="42" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="27" t="s">
+      <c r="A42" s="134" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="28"/>
-      <c r="C42" s="29">
+      <c r="B42" s="135"/>
+      <c r="C42" s="136">
         <f>'Other Details'!G2</f>
         <v>0</v>
       </c>
-      <c r="D42" s="30"/>
-      <c r="E42" s="30"/>
-      <c r="F42" s="30"/>
-      <c r="G42" s="30"/>
-      <c r="H42" s="30"/>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
-      <c r="K42" s="30"/>
-      <c r="L42" s="30"/>
-      <c r="M42" s="31"/>
+      <c r="D42" s="137"/>
+      <c r="E42" s="137"/>
+      <c r="F42" s="137"/>
+      <c r="G42" s="137"/>
+      <c r="H42" s="137"/>
+      <c r="I42" s="137"/>
+      <c r="J42" s="137"/>
+      <c r="K42" s="137"/>
+      <c r="L42" s="137"/>
+      <c r="M42" s="138"/>
       <c r="N42" s="13"/>
       <c r="O42" s="13"/>
       <c r="P42" s="13"/>
       <c r="Q42" s="14"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A43" s="32" t="s">
+      <c r="A43" s="139" t="s">
         <v>34</v>
       </c>
-      <c r="B43" s="32"/>
-      <c r="C43" s="32"/>
-      <c r="D43" s="32"/>
-      <c r="E43" s="32"/>
-      <c r="F43" s="32"/>
-      <c r="G43" s="32"/>
-      <c r="H43" s="32"/>
-      <c r="I43" s="32"/>
-      <c r="J43" s="32"/>
-      <c r="K43" s="32"/>
-      <c r="L43" s="32"/>
-      <c r="M43" s="32"/>
-      <c r="N43" s="32"/>
-      <c r="O43" s="32"/>
-      <c r="P43" s="32"/>
-      <c r="Q43" s="32"/>
+      <c r="B43" s="139"/>
+      <c r="C43" s="139"/>
+      <c r="D43" s="139"/>
+      <c r="E43" s="139"/>
+      <c r="F43" s="139"/>
+      <c r="G43" s="139"/>
+      <c r="H43" s="139"/>
+      <c r="I43" s="139"/>
+      <c r="J43" s="139"/>
+      <c r="K43" s="139"/>
+      <c r="L43" s="139"/>
+      <c r="M43" s="139"/>
+      <c r="N43" s="139"/>
+      <c r="O43" s="139"/>
+      <c r="P43" s="139"/>
+      <c r="Q43" s="139"/>
     </row>
   </sheetData>
   <mergeCells count="142">
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="H2:Q2"/>
-    <mergeCell ref="A3:Q3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="G4:M4"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="G5:M5"/>
-    <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="A6:Q6"/>
-    <mergeCell ref="A7:Q7"/>
-    <mergeCell ref="A8:C9"/>
-    <mergeCell ref="D8:G9"/>
-    <mergeCell ref="H8:M9"/>
-    <mergeCell ref="N8:Q9"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="H17:M17"/>
-    <mergeCell ref="A18:Q18"/>
-    <mergeCell ref="A19:O19"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A12:Q12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="H14:M14"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:M42"/>
+    <mergeCell ref="A43:Q43"/>
+    <mergeCell ref="N38:O38"/>
+    <mergeCell ref="A39:M39"/>
+    <mergeCell ref="A40:M40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="C41:M41"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="L38:M38"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="L37:M37"/>
+    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="L36:M36"/>
+    <mergeCell ref="N34:O34"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="N35:O35"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="N32:O32"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="A28:Q28"/>
+    <mergeCell ref="A29:O29"/>
+    <mergeCell ref="A30:C31"/>
+    <mergeCell ref="D30:E31"/>
+    <mergeCell ref="F30:G31"/>
+    <mergeCell ref="H30:I31"/>
+    <mergeCell ref="J30:K31"/>
+    <mergeCell ref="L30:M31"/>
+    <mergeCell ref="N30:O31"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="N26:O26"/>
     <mergeCell ref="N20:O21"/>
     <mergeCell ref="A22:C27"/>
     <mergeCell ref="D22:E22"/>
@@ -3000,94 +3060,42 @@
     <mergeCell ref="N25:O25"/>
     <mergeCell ref="H23:I23"/>
     <mergeCell ref="J23:K23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="A28:Q28"/>
-    <mergeCell ref="A29:O29"/>
-    <mergeCell ref="A30:C31"/>
-    <mergeCell ref="D30:E31"/>
-    <mergeCell ref="F30:G31"/>
-    <mergeCell ref="H30:I31"/>
-    <mergeCell ref="J30:K31"/>
-    <mergeCell ref="L30:M31"/>
-    <mergeCell ref="N30:O31"/>
-    <mergeCell ref="N32:O32"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="N33:O33"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="N34:O34"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="J35:K35"/>
-    <mergeCell ref="L35:M35"/>
-    <mergeCell ref="N35:O35"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="L34:M34"/>
-    <mergeCell ref="N36:O36"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="L37:M37"/>
-    <mergeCell ref="N37:O37"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="J36:K36"/>
-    <mergeCell ref="L36:M36"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C42:M42"/>
-    <mergeCell ref="A43:Q43"/>
-    <mergeCell ref="N38:O38"/>
-    <mergeCell ref="A39:M39"/>
-    <mergeCell ref="A40:M40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:M41"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="L38:M38"/>
+    <mergeCell ref="A18:Q18"/>
+    <mergeCell ref="A19:O19"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:Q12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="H14:M14"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="A6:Q6"/>
+    <mergeCell ref="A7:Q7"/>
+    <mergeCell ref="A8:C9"/>
+    <mergeCell ref="D8:G9"/>
+    <mergeCell ref="H8:M9"/>
+    <mergeCell ref="N8:Q9"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="H17:M17"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="H2:Q2"/>
+    <mergeCell ref="A3:Q3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="G4:M4"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="G5:M5"/>
+    <mergeCell ref="N5:Q5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="79" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updates to PSR template for improved printing
</commit_message>
<xml_diff>
--- a/temporary-psr-generation/psr-template.xlsx
+++ b/temporary-psr-generation/psr-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmgiven/Developer/gov.ct/ecis-data-migration/temporary-psr-generation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2772405-0A28-9145-B71A-463FEB695906}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991C4275-DF44-1749-878F-F9FC91316A0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5480" yWindow="820" windowWidth="23020" windowHeight="20520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -360,7 +360,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -369,19 +369,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD8E5BC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -405,13 +393,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="43"/>
+        <fgColor rgb="FF76933B"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF76933B"/>
+        <fgColor rgb="FFEFF4E4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFE6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -925,9 +919,6 @@
   </cellStyleXfs>
   <cellXfs count="164">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -971,19 +962,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -999,49 +984,235 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1053,362 +1224,185 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="8" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="8" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="8" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1416,6 +1410,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFFE6"/>
+      <color rgb="FFEFF4E4"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1730,7 +1730,7 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+      <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1746,1296 +1746,1244 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="110" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="38"/>
+      <c r="B1" s="111"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
+      <c r="I1" s="111"/>
+      <c r="J1" s="111"/>
+      <c r="K1" s="111"/>
+      <c r="L1" s="111"/>
+      <c r="M1" s="111"/>
+      <c r="N1" s="111"/>
+      <c r="O1" s="111"/>
+      <c r="P1" s="111"/>
+      <c r="Q1" s="112"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="134" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="40">
+      <c r="B2" s="134"/>
+      <c r="C2" s="134"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="134"/>
+      <c r="F2" s="134"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="135">
         <f>'Other Details'!A2</f>
         <v>0</v>
       </c>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="41"/>
+      <c r="I2" s="135"/>
+      <c r="J2" s="135"/>
+      <c r="K2" s="135"/>
+      <c r="L2" s="135"/>
+      <c r="M2" s="135"/>
+      <c r="N2" s="135"/>
+      <c r="O2" s="135"/>
+      <c r="P2" s="135"/>
+      <c r="Q2" s="136"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="42"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
-      <c r="O3" s="43"/>
-      <c r="P3" s="43"/>
-      <c r="Q3" s="44"/>
+      <c r="A3" s="101"/>
+      <c r="B3" s="102"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="102"/>
+      <c r="I3" s="102"/>
+      <c r="J3" s="102"/>
+      <c r="K3" s="102"/>
+      <c r="L3" s="102"/>
+      <c r="M3" s="102"/>
+      <c r="N3" s="102"/>
+      <c r="O3" s="102"/>
+      <c r="P3" s="102"/>
+      <c r="Q3" s="103"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="113" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="47">
+      <c r="B4" s="114"/>
+      <c r="C4" s="114"/>
+      <c r="D4" s="114"/>
+      <c r="E4" s="114"/>
+      <c r="F4" s="114"/>
+      <c r="G4" s="148">
         <f>'Other Details'!B2</f>
         <v>0</v>
       </c>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
-      <c r="M4" s="49"/>
-      <c r="Q4" s="2"/>
+      <c r="H4" s="149"/>
+      <c r="I4" s="149"/>
+      <c r="J4" s="149"/>
+      <c r="K4" s="149"/>
+      <c r="L4" s="149"/>
+      <c r="M4" s="150"/>
+      <c r="Q4" s="1"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="113" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="47">
+      <c r="B5" s="114"/>
+      <c r="C5" s="114"/>
+      <c r="D5" s="114"/>
+      <c r="E5" s="114"/>
+      <c r="F5" s="114"/>
+      <c r="G5" s="148">
         <f>'Other Details'!C2</f>
         <v>0</v>
       </c>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="48"/>
-      <c r="L5" s="48"/>
-      <c r="M5" s="49"/>
-      <c r="N5" s="50"/>
-      <c r="O5" s="50"/>
-      <c r="P5" s="50"/>
-      <c r="Q5" s="51"/>
+      <c r="H5" s="149"/>
+      <c r="I5" s="149"/>
+      <c r="J5" s="149"/>
+      <c r="K5" s="149"/>
+      <c r="L5" s="149"/>
+      <c r="M5" s="150"/>
+      <c r="N5" s="115"/>
+      <c r="O5" s="115"/>
+      <c r="P5" s="115"/>
+      <c r="Q5" s="116"/>
     </row>
     <row r="6" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="42"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
-      <c r="L6" s="43"/>
-      <c r="M6" s="43"/>
-      <c r="N6" s="43"/>
-      <c r="O6" s="43"/>
-      <c r="P6" s="43"/>
-      <c r="Q6" s="44"/>
+      <c r="A6" s="101"/>
+      <c r="B6" s="102"/>
+      <c r="C6" s="102"/>
+      <c r="D6" s="102"/>
+      <c r="E6" s="102"/>
+      <c r="F6" s="102"/>
+      <c r="G6" s="102"/>
+      <c r="H6" s="102"/>
+      <c r="I6" s="102"/>
+      <c r="J6" s="102"/>
+      <c r="K6" s="102"/>
+      <c r="L6" s="102"/>
+      <c r="M6" s="102"/>
+      <c r="N6" s="102"/>
+      <c r="O6" s="102"/>
+      <c r="P6" s="102"/>
+      <c r="Q6" s="103"/>
     </row>
     <row r="7" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="53"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="53"/>
-      <c r="M7" s="53"/>
-      <c r="N7" s="53"/>
-      <c r="O7" s="53"/>
-      <c r="P7" s="53"/>
-      <c r="Q7" s="54"/>
+      <c r="B7" s="66"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="66"/>
+      <c r="J7" s="66"/>
+      <c r="K7" s="66"/>
+      <c r="L7" s="66"/>
+      <c r="M7" s="66"/>
+      <c r="N7" s="66"/>
+      <c r="O7" s="66"/>
+      <c r="P7" s="66"/>
+      <c r="Q7" s="67"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="55"/>
-      <c r="B8" s="56"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="59" t="s">
+      <c r="A8" s="117"/>
+      <c r="B8" s="118"/>
+      <c r="C8" s="118"/>
+      <c r="D8" s="119" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="60"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="61"/>
-      <c r="H8" s="59" t="s">
+      <c r="E8" s="120"/>
+      <c r="F8" s="120"/>
+      <c r="G8" s="121"/>
+      <c r="H8" s="119" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="60"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="60"/>
-      <c r="L8" s="60"/>
-      <c r="M8" s="61"/>
-      <c r="N8" s="60" t="s">
+      <c r="I8" s="120"/>
+      <c r="J8" s="120"/>
+      <c r="K8" s="120"/>
+      <c r="L8" s="120"/>
+      <c r="M8" s="121"/>
+      <c r="N8" s="120" t="s">
         <v>37</v>
       </c>
-      <c r="O8" s="60"/>
-      <c r="P8" s="60"/>
-      <c r="Q8" s="61"/>
+      <c r="O8" s="120"/>
+      <c r="P8" s="120"/>
+      <c r="Q8" s="121"/>
     </row>
     <row r="9" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="57"/>
-      <c r="B9" s="58"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="64"/>
-      <c r="H9" s="62"/>
-      <c r="I9" s="63"/>
-      <c r="J9" s="63"/>
-      <c r="K9" s="63"/>
-      <c r="L9" s="63"/>
-      <c r="M9" s="64"/>
-      <c r="N9" s="63"/>
-      <c r="O9" s="63"/>
-      <c r="P9" s="63"/>
-      <c r="Q9" s="64"/>
+      <c r="A9" s="122"/>
+      <c r="B9" s="123"/>
+      <c r="C9" s="123"/>
+      <c r="D9" s="124"/>
+      <c r="E9" s="125"/>
+      <c r="F9" s="125"/>
+      <c r="G9" s="126"/>
+      <c r="H9" s="124"/>
+      <c r="I9" s="125"/>
+      <c r="J9" s="125"/>
+      <c r="K9" s="125"/>
+      <c r="L9" s="125"/>
+      <c r="M9" s="126"/>
+      <c r="N9" s="125"/>
+      <c r="O9" s="125"/>
+      <c r="P9" s="125"/>
+      <c r="Q9" s="126"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="88"/>
-      <c r="B10" s="89"/>
-      <c r="C10" s="90"/>
-      <c r="D10" s="91" t="s">
+      <c r="A10" s="96"/>
+      <c r="B10" s="97"/>
+      <c r="C10" s="98"/>
+      <c r="D10" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="77"/>
-      <c r="F10" s="77" t="s">
+      <c r="E10" s="83"/>
+      <c r="F10" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="78"/>
-      <c r="H10" s="91" t="s">
+      <c r="G10" s="84"/>
+      <c r="H10" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="I10" s="77"/>
-      <c r="J10" s="77"/>
-      <c r="K10" s="77" t="s">
+      <c r="I10" s="83"/>
+      <c r="J10" s="83"/>
+      <c r="K10" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="L10" s="77"/>
-      <c r="M10" s="78"/>
-      <c r="N10" s="92" t="s">
+      <c r="L10" s="83"/>
+      <c r="M10" s="84"/>
+      <c r="N10" s="100" t="s">
         <v>36</v>
       </c>
-      <c r="O10" s="77"/>
-      <c r="P10" s="77" t="s">
+      <c r="O10" s="83"/>
+      <c r="P10" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="Q10" s="78"/>
+      <c r="Q10" s="84"/>
     </row>
     <row r="11" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="79"/>
-      <c r="B11" s="80"/>
-      <c r="C11" s="81"/>
-      <c r="D11" s="7" t="s">
+      <c r="A11" s="85"/>
+      <c r="B11" s="86"/>
+      <c r="C11" s="87"/>
+      <c r="D11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="18"/>
-      <c r="J11" s="15" t="s">
+      <c r="I11" s="17"/>
+      <c r="J11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="K11" s="15" t="s">
+      <c r="K11" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="L11" s="18"/>
-      <c r="M11" s="16" t="s">
+      <c r="L11" s="17"/>
+      <c r="M11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="N11" s="19" t="s">
+      <c r="N11" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="O11" s="15" t="s">
+      <c r="O11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="P11" s="15" t="s">
+      <c r="P11" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="Q11" s="16" t="s">
+      <c r="Q11" s="15" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="82"/>
-      <c r="B12" s="83"/>
-      <c r="C12" s="83"/>
-      <c r="D12" s="83"/>
-      <c r="E12" s="83"/>
-      <c r="F12" s="83"/>
-      <c r="G12" s="83"/>
-      <c r="H12" s="83"/>
-      <c r="I12" s="83"/>
-      <c r="J12" s="83"/>
-      <c r="K12" s="83"/>
-      <c r="L12" s="83"/>
-      <c r="M12" s="83"/>
-      <c r="N12" s="83"/>
-      <c r="O12" s="83"/>
-      <c r="P12" s="83"/>
-      <c r="Q12" s="84"/>
+      <c r="A12" s="88"/>
+      <c r="B12" s="89"/>
+      <c r="C12" s="89"/>
+      <c r="D12" s="89"/>
+      <c r="E12" s="89"/>
+      <c r="F12" s="89"/>
+      <c r="G12" s="89"/>
+      <c r="H12" s="89"/>
+      <c r="I12" s="89"/>
+      <c r="J12" s="89"/>
+      <c r="K12" s="89"/>
+      <c r="L12" s="89"/>
+      <c r="M12" s="89"/>
+      <c r="N12" s="89"/>
+      <c r="O12" s="89"/>
+      <c r="P12" s="89"/>
+      <c r="Q12" s="90"/>
     </row>
     <row r="13" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="65" t="s">
+      <c r="A13" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="66"/>
-      <c r="C13" s="67"/>
-      <c r="D13" s="20" t="str">
+      <c r="B13" s="92"/>
+      <c r="C13" s="93"/>
+      <c r="D13" s="137" t="str">
         <f t="array" ref="D13">IFERROR(INDEX(Spaces!$E:$E,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Acc.")*(Spaces!$D:$D="Standard"),0)),"")</f>
         <v/>
       </c>
-      <c r="E13" s="21" t="str">
+      <c r="E13" s="138" t="str">
         <f t="array" ref="E13">IFERROR(INDEX(Spaces!$E:$E,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Una")*(Spaces!$D:$D="Standard"),0)),"")</f>
         <v/>
       </c>
-      <c r="F13" s="21" t="str">
+      <c r="F13" s="138" t="str">
         <f t="array" ref="F13">IFERROR(INDEX(Spaces!$E:$E,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Acc.")*(Spaces!$D:$D="Standard"),0)),"")</f>
         <v/>
       </c>
-      <c r="G13" s="1" t="str">
+      <c r="G13" s="139" t="str">
         <f t="array" ref="G13">IFERROR(INDEX(Spaces!$E:$E,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Una")*(Spaces!$D:$D="Standard"),0)),"")</f>
         <v/>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="5">
         <v>165.32</v>
       </c>
-      <c r="I13" s="17"/>
-      <c r="J13" s="22">
+      <c r="I13" s="16"/>
+      <c r="J13" s="19">
         <v>126.59</v>
       </c>
-      <c r="K13" s="22">
+      <c r="K13" s="19">
         <v>57.85</v>
       </c>
-      <c r="L13" s="17"/>
-      <c r="M13" s="25">
+      <c r="L13" s="16"/>
+      <c r="M13" s="22">
         <v>44.2</v>
       </c>
-      <c r="N13" s="20" t="str">
+      <c r="N13" s="137" t="str">
         <f t="array" ref="N13">IFERROR(INDEX(Spaces!$E:$E,MATCH(1,(Spaces!$A:$A="School-age")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Acc.")*(Spaces!$D:$D="Standard"),0)),"")</f>
         <v/>
       </c>
-      <c r="O13" s="21" t="str">
+      <c r="O13" s="138" t="str">
         <f t="array" ref="O13">IFERROR(INDEX(Spaces!$E:$E,MATCH(1,(Spaces!$A:$A="School-age")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Una")*(Spaces!$D:$D="Standard"),0)),"")</f>
         <v/>
       </c>
-      <c r="P13" s="21" t="str">
+      <c r="P13" s="138" t="str">
         <f t="array" ref="P13">IFERROR(INDEX(Spaces!$E:$E,MATCH(1,(Spaces!$A:$A="School-age")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Acc.")*(Spaces!$D:$D="Standard"),0)),"")</f>
         <v/>
       </c>
-      <c r="Q13" s="1" t="str">
+      <c r="Q13" s="139" t="str">
         <f t="array" ref="Q13">IFERROR(INDEX(Spaces!$E:$E,MATCH(1,(Spaces!$A:$A="School-age")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Una")*(Spaces!$D:$D="Standard"),0)),"")</f>
         <v/>
       </c>
     </row>
     <row r="14" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="65" t="s">
+      <c r="A14" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="66"/>
-      <c r="C14" s="67"/>
-      <c r="D14" s="20" t="str">
+      <c r="B14" s="92"/>
+      <c r="C14" s="93"/>
+      <c r="D14" s="137" t="str">
         <f t="array" ref="D14">IFERROR(INDEX(Spaces!$E:$E,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Acc.")*(Spaces!$D:$D="Title I"),0)),"")</f>
         <v/>
       </c>
-      <c r="E14" s="21" t="str">
+      <c r="E14" s="138" t="str">
         <f t="array" ref="E14">IFERROR(INDEX(Spaces!$E:$E,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Una")*(Spaces!$D:$D="Title I"),0)),"")</f>
         <v/>
       </c>
-      <c r="F14" s="21" t="str">
+      <c r="F14" s="138" t="str">
         <f t="array" ref="F14">IFERROR(INDEX(Spaces!$E:$E,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Acc.")*(Spaces!$D:$D="Title I"),0)),"")</f>
         <v/>
       </c>
-      <c r="G14" s="1" t="str">
+      <c r="G14" s="139" t="str">
         <f t="array" ref="G14">IFERROR(INDEX(Spaces!$E:$E,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Una")*(Spaces!$D:$D="Title I"),0)),"")</f>
         <v/>
       </c>
-      <c r="H14" s="85"/>
-      <c r="I14" s="86"/>
-      <c r="J14" s="86"/>
-      <c r="K14" s="86"/>
-      <c r="L14" s="86"/>
-      <c r="M14" s="87"/>
-      <c r="N14" s="20" t="str">
+      <c r="H14" s="51"/>
+      <c r="I14" s="94"/>
+      <c r="J14" s="94"/>
+      <c r="K14" s="94"/>
+      <c r="L14" s="94"/>
+      <c r="M14" s="95"/>
+      <c r="N14" s="137" t="str">
         <f t="array" ref="N14">IFERROR(INDEX(Spaces!$E:$E,MATCH(1,(Spaces!$A:$A="School-age")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Acc.")*(Spaces!$D:$D="Title I"),0)),"")</f>
         <v/>
       </c>
-      <c r="O14" s="21" t="str">
+      <c r="O14" s="138" t="str">
         <f t="array" ref="O14">IFERROR(INDEX(Spaces!$E:$E,MATCH(1,(Spaces!$A:$A="School-age")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Una")*(Spaces!$D:$D="Title I"),0)),"")</f>
         <v/>
       </c>
-      <c r="P14" s="21" t="str">
+      <c r="P14" s="138" t="str">
         <f t="array" ref="P14">IFERROR(INDEX(Spaces!$E:$E,MATCH(1,(Spaces!$A:$A="School-age")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Acc.")*(Spaces!$D:$D="Title I"),0)),"")</f>
         <v/>
       </c>
-      <c r="Q14" s="1" t="str">
+      <c r="Q14" s="139" t="str">
         <f t="array" ref="Q14">IFERROR(INDEX(Spaces!$E:$E,MATCH(1,(Spaces!$A:$A="School-age")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Una")*(Spaces!$D:$D="Title I"),0)),"")</f>
         <v/>
       </c>
     </row>
     <row r="15" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="65" t="s">
+      <c r="A15" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="66"/>
-      <c r="C15" s="67"/>
-      <c r="D15" s="27" t="str">
+      <c r="B15" s="92"/>
+      <c r="C15" s="93"/>
+      <c r="D15" s="140" t="str">
         <f t="array" ref="D15">IFERROR(INDEX(Spaces!$F:$F,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Acc."),0)),"")</f>
         <v/>
       </c>
-      <c r="E15" s="28" t="str">
+      <c r="E15" s="141" t="str">
         <f t="array" ref="E15">IFERROR(INDEX(Spaces!$F:$F,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Una"),0)),"")</f>
         <v/>
       </c>
-      <c r="F15" s="28" t="str">
+      <c r="F15" s="141" t="str">
         <f t="array" ref="F15">IFERROR(INDEX(Spaces!$F:$F,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Acc."),0)),"")</f>
         <v/>
       </c>
-      <c r="G15" s="29" t="str">
+      <c r="G15" s="142" t="str">
         <f t="array" ref="G15">IFERROR(INDEX(Spaces!$F:$F,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Una"),0)),"")</f>
         <v/>
       </c>
-      <c r="H15" s="27" t="str">
+      <c r="H15" s="140" t="str">
         <f t="array" ref="H15">IFERROR(INDEX(Spaces!$F:$F,MATCH(1,(Spaces!$A:$A="Preschool")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Acc."),0)),"")</f>
         <v/>
       </c>
-      <c r="I15" s="30"/>
-      <c r="J15" s="28" t="str">
+      <c r="I15" s="24"/>
+      <c r="J15" s="141" t="str">
         <f t="array" ref="J15">IFERROR(INDEX(Spaces!$F:$F,MATCH(1,(Spaces!$A:$A="Preschool")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Una"),0)),"")</f>
         <v/>
       </c>
-      <c r="K15" s="28" t="str">
+      <c r="K15" s="141" t="str">
         <f t="array" ref="K15">IFERROR(INDEX(Spaces!$F:$F,MATCH(1,(Spaces!$A:$A="Preschool")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Acc."),0)),"")</f>
         <v/>
       </c>
-      <c r="L15" s="30"/>
-      <c r="M15" s="29" t="str">
+      <c r="L15" s="24"/>
+      <c r="M15" s="142" t="str">
         <f t="array" ref="M15">IFERROR(INDEX(Spaces!$F:$F,MATCH(1,(Spaces!$A:$A="Preschool")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Una"),0)),"")</f>
         <v/>
       </c>
-      <c r="N15" s="31" t="str">
+      <c r="N15" s="146" t="str">
         <f t="array" ref="N15">IFERROR(INDEX(Spaces!$F:$F,MATCH(1,(Spaces!$A:$A="School-age")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Acc."),0)),"")</f>
         <v/>
       </c>
-      <c r="O15" s="28" t="str">
+      <c r="O15" s="141" t="str">
         <f t="array" ref="O15">IFERROR(INDEX(Spaces!$F:$F,MATCH(1,(Spaces!$A:$A="School-age")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Una"),0)),"")</f>
         <v/>
       </c>
-      <c r="P15" s="28" t="str">
+      <c r="P15" s="141" t="str">
         <f t="array" ref="P15">IFERROR(INDEX(Spaces!$F:$F,MATCH(1,(Spaces!$A:$A="School-age")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Acc."),0)),"")</f>
         <v/>
       </c>
-      <c r="Q15" s="29" t="str">
+      <c r="Q15" s="142" t="str">
         <f t="array" ref="Q15">IFERROR(INDEX(Spaces!$F:$F,MATCH(1,(Spaces!$A:$A="School-age")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Una"),0)),"")</f>
         <v/>
       </c>
     </row>
     <row r="16" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="65" t="s">
+      <c r="A16" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="66"/>
-      <c r="C16" s="67"/>
-      <c r="D16" s="27" t="str">
+      <c r="B16" s="92"/>
+      <c r="C16" s="93"/>
+      <c r="D16" s="140" t="str">
         <f t="array" ref="D16">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Acc.")*(Spaces!$D:$D="Standard"),0)),"")</f>
         <v/>
       </c>
-      <c r="E16" s="28" t="str">
+      <c r="E16" s="141" t="str">
         <f t="array" ref="E16">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Una")*(Spaces!$D:$D="Standard"),0)),"")</f>
         <v/>
       </c>
-      <c r="F16" s="28" t="str">
+      <c r="F16" s="141" t="str">
         <f t="array" ref="F16">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Acc.")*(Spaces!$D:$D="Standard"),0)),"")</f>
         <v/>
       </c>
-      <c r="G16" s="29" t="str">
+      <c r="G16" s="142" t="str">
         <f t="array" ref="G16">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Una")*(Spaces!$D:$D="Standard"),0)),"")</f>
         <v/>
       </c>
-      <c r="H16" s="27" t="str">
+      <c r="H16" s="140" t="str">
         <f t="array" ref="H16">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="Preschool")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Acc."),0)),"")</f>
         <v/>
       </c>
-      <c r="I16" s="30"/>
-      <c r="J16" s="28" t="str">
+      <c r="I16" s="24"/>
+      <c r="J16" s="141" t="str">
         <f t="array" ref="J16">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="Preschool")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Una"),0)),"")</f>
         <v/>
       </c>
-      <c r="K16" s="28" t="str">
+      <c r="K16" s="141" t="str">
         <f t="array" ref="K16">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="Preschool")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Acc."),0)),"")</f>
         <v/>
       </c>
-      <c r="L16" s="30"/>
-      <c r="M16" s="29" t="str">
+      <c r="L16" s="24"/>
+      <c r="M16" s="142" t="str">
         <f t="array" ref="M16">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="Preschool")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Una"),0)),"")</f>
         <v/>
       </c>
-      <c r="N16" s="31" t="str">
+      <c r="N16" s="146" t="str">
         <f t="array" ref="N16">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="School-age")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Acc.")*(Spaces!$D:$D="Standard"),0)),"")</f>
         <v/>
       </c>
-      <c r="O16" s="28" t="str">
+      <c r="O16" s="141" t="str">
         <f t="array" ref="O16">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="School-age")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Una")*(Spaces!$D:$D="Standard"),0)),"")</f>
         <v/>
       </c>
-      <c r="P16" s="28" t="str">
+      <c r="P16" s="141" t="str">
         <f t="array" ref="P16">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="School-age")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Acc.")*(Spaces!$D:$D="Standard"),0)),"")</f>
         <v/>
       </c>
-      <c r="Q16" s="29" t="str">
+      <c r="Q16" s="142" t="str">
         <f t="array" ref="Q16">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="School-age")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Una")*(Spaces!$D:$D="Standard"),0)),"")</f>
         <v/>
       </c>
     </row>
     <row r="17" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="68" t="s">
+      <c r="A17" s="104" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="69"/>
-      <c r="C17" s="70"/>
-      <c r="D17" s="32" t="str">
+      <c r="B17" s="105"/>
+      <c r="C17" s="106"/>
+      <c r="D17" s="143" t="str">
         <f t="array" ref="D17">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Acc.")*(Spaces!$D:$D="Title I"),0)),"")</f>
         <v/>
       </c>
-      <c r="E17" s="33" t="str">
+      <c r="E17" s="144" t="str">
         <f t="array" ref="E17">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Una")*(Spaces!$D:$D="Title I"),0)),"")</f>
         <v/>
       </c>
-      <c r="F17" s="33" t="str">
+      <c r="F17" s="144" t="str">
         <f t="array" ref="F17">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Acc.")*(Spaces!$D:$D="Title I"),0)),"")</f>
         <v/>
       </c>
-      <c r="G17" s="34" t="str">
+      <c r="G17" s="145" t="str">
         <f t="array" ref="G17">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="Infant/Toddler")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Una")*(Spaces!$D:$D="Title I"),0)),"")</f>
         <v/>
       </c>
-      <c r="H17" s="71"/>
-      <c r="I17" s="72"/>
-      <c r="J17" s="72"/>
-      <c r="K17" s="72"/>
-      <c r="L17" s="72"/>
-      <c r="M17" s="73"/>
-      <c r="N17" s="35" t="str">
+      <c r="H17" s="107"/>
+      <c r="I17" s="108"/>
+      <c r="J17" s="108"/>
+      <c r="K17" s="108"/>
+      <c r="L17" s="108"/>
+      <c r="M17" s="109"/>
+      <c r="N17" s="147" t="str">
         <f t="array" ref="N17">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="School-age")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Acc.")*(Spaces!$D:$D="Title I"),0)),"")</f>
         <v/>
       </c>
-      <c r="O17" s="33" t="str">
+      <c r="O17" s="144" t="str">
         <f t="array" ref="O17">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="School-age")*(Spaces!$B:$B="FT")*(Spaces!$C:$C="Una")*(Spaces!$D:$D="Title I"),0)),"")</f>
         <v/>
       </c>
-      <c r="P17" s="33" t="str">
+      <c r="P17" s="144" t="str">
         <f t="array" ref="P17">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="School-age")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Acc.")*(Spaces!$D:$D="Title I"),0)),"")</f>
         <v/>
       </c>
-      <c r="Q17" s="34" t="str">
+      <c r="Q17" s="145" t="str">
         <f t="array" ref="Q17">IFERROR(INDEX(Spaces!$G:$G,MATCH(1,(Spaces!$A:$A="School-age")*(Spaces!$B:$B="PT")*(Spaces!$C:$C="Una")*(Spaces!$D:$D="Title I"),0)),"")</f>
         <v/>
       </c>
     </row>
     <row r="18" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="74"/>
-      <c r="B18" s="75"/>
-      <c r="C18" s="75"/>
-      <c r="D18" s="75"/>
-      <c r="E18" s="75"/>
-      <c r="F18" s="75"/>
-      <c r="G18" s="75"/>
-      <c r="H18" s="75"/>
-      <c r="I18" s="75"/>
-      <c r="J18" s="75"/>
-      <c r="K18" s="75"/>
-      <c r="L18" s="75"/>
-      <c r="M18" s="75"/>
-      <c r="N18" s="75"/>
-      <c r="O18" s="75"/>
-      <c r="P18" s="75"/>
-      <c r="Q18" s="76"/>
+      <c r="A18" s="62"/>
+      <c r="B18" s="63"/>
+      <c r="C18" s="63"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="63"/>
+      <c r="F18" s="63"/>
+      <c r="G18" s="63"/>
+      <c r="H18" s="63"/>
+      <c r="I18" s="63"/>
+      <c r="J18" s="63"/>
+      <c r="K18" s="63"/>
+      <c r="L18" s="63"/>
+      <c r="M18" s="63"/>
+      <c r="N18" s="63"/>
+      <c r="O18" s="63"/>
+      <c r="P18" s="63"/>
+      <c r="Q18" s="64"/>
     </row>
     <row r="19" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="52" t="s">
+      <c r="A19" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="53"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="53"/>
-      <c r="G19" s="53"/>
-      <c r="H19" s="53"/>
-      <c r="I19" s="53"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="53"/>
-      <c r="L19" s="53"/>
-      <c r="M19" s="53"/>
-      <c r="N19" s="53"/>
-      <c r="O19" s="54"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="4"/>
+      <c r="B19" s="66"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="66"/>
+      <c r="G19" s="66"/>
+      <c r="H19" s="66"/>
+      <c r="I19" s="66"/>
+      <c r="J19" s="66"/>
+      <c r="K19" s="66"/>
+      <c r="L19" s="66"/>
+      <c r="M19" s="66"/>
+      <c r="N19" s="66"/>
+      <c r="O19" s="67"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="3"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A20" s="55"/>
-      <c r="B20" s="56"/>
-      <c r="C20" s="108"/>
-      <c r="D20" s="59" t="s">
+      <c r="A20" s="117"/>
+      <c r="B20" s="118"/>
+      <c r="C20" s="127"/>
+      <c r="D20" s="119" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="61"/>
-      <c r="F20" s="60" t="s">
+      <c r="E20" s="121"/>
+      <c r="F20" s="120" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="61"/>
-      <c r="H20" s="59" t="s">
+      <c r="G20" s="121"/>
+      <c r="H20" s="119" t="s">
         <v>17</v>
       </c>
-      <c r="I20" s="60"/>
-      <c r="J20" s="59" t="s">
+      <c r="I20" s="120"/>
+      <c r="J20" s="119" t="s">
         <v>15</v>
       </c>
-      <c r="K20" s="61"/>
-      <c r="L20" s="60" t="s">
+      <c r="K20" s="121"/>
+      <c r="L20" s="120" t="s">
         <v>16</v>
       </c>
-      <c r="M20" s="61"/>
-      <c r="N20" s="59" t="s">
+      <c r="M20" s="121"/>
+      <c r="N20" s="119" t="s">
         <v>17</v>
       </c>
-      <c r="O20" s="61"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="4"/>
+      <c r="O20" s="121"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="3"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A21" s="109"/>
-      <c r="B21" s="110"/>
-      <c r="C21" s="111"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="63"/>
-      <c r="G21" s="64"/>
-      <c r="H21" s="62"/>
-      <c r="I21" s="63"/>
-      <c r="J21" s="62"/>
-      <c r="K21" s="64"/>
-      <c r="L21" s="63"/>
-      <c r="M21" s="64"/>
-      <c r="N21" s="62"/>
-      <c r="O21" s="64"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="4"/>
+      <c r="A21" s="128"/>
+      <c r="B21" s="129"/>
+      <c r="C21" s="130"/>
+      <c r="D21" s="124"/>
+      <c r="E21" s="126"/>
+      <c r="F21" s="125"/>
+      <c r="G21" s="126"/>
+      <c r="H21" s="124"/>
+      <c r="I21" s="125"/>
+      <c r="J21" s="124"/>
+      <c r="K21" s="126"/>
+      <c r="L21" s="125"/>
+      <c r="M21" s="126"/>
+      <c r="N21" s="124"/>
+      <c r="O21" s="126"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="3"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A22" s="93"/>
-      <c r="B22" s="94"/>
-      <c r="C22" s="95"/>
-      <c r="D22" s="102">
+      <c r="A22" s="74"/>
+      <c r="B22" s="75"/>
+      <c r="C22" s="76"/>
+      <c r="D22" s="70">
         <v>1</v>
       </c>
-      <c r="E22" s="103"/>
-      <c r="F22" s="104">
+      <c r="E22" s="71"/>
+      <c r="F22" s="68">
         <v>24280</v>
       </c>
-      <c r="G22" s="105"/>
-      <c r="H22" s="106">
+      <c r="G22" s="69"/>
+      <c r="H22" s="151">
         <f>'Family Income Groupings'!C2</f>
         <v>0</v>
       </c>
-      <c r="I22" s="106"/>
-      <c r="J22" s="102">
+      <c r="I22" s="151"/>
+      <c r="J22" s="70">
         <v>7</v>
       </c>
-      <c r="K22" s="103"/>
-      <c r="L22" s="104">
+      <c r="K22" s="71"/>
+      <c r="L22" s="68">
         <v>76120</v>
       </c>
-      <c r="M22" s="105"/>
-      <c r="N22" s="107">
+      <c r="M22" s="69"/>
+      <c r="N22" s="152">
         <f>'Family Income Groupings'!C8</f>
         <v>0</v>
       </c>
-      <c r="O22" s="107"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="4"/>
+      <c r="O22" s="152"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="3"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A23" s="96"/>
-      <c r="B23" s="97"/>
-      <c r="C23" s="98"/>
-      <c r="D23" s="102">
+      <c r="A23" s="77"/>
+      <c r="B23" s="78"/>
+      <c r="C23" s="79"/>
+      <c r="D23" s="70">
         <v>2</v>
       </c>
-      <c r="E23" s="103"/>
-      <c r="F23" s="104">
+      <c r="E23" s="71"/>
+      <c r="F23" s="68">
         <v>32920</v>
       </c>
-      <c r="G23" s="105"/>
-      <c r="H23" s="106">
+      <c r="G23" s="69"/>
+      <c r="H23" s="151">
         <f>'Family Income Groupings'!C3</f>
         <v>0</v>
       </c>
-      <c r="I23" s="106"/>
-      <c r="J23" s="102">
+      <c r="I23" s="151"/>
+      <c r="J23" s="70">
         <v>8</v>
       </c>
-      <c r="K23" s="103"/>
-      <c r="L23" s="104">
+      <c r="K23" s="71"/>
+      <c r="L23" s="68">
         <v>84760</v>
       </c>
-      <c r="M23" s="105"/>
-      <c r="N23" s="107">
+      <c r="M23" s="69"/>
+      <c r="N23" s="152">
         <f>'Family Income Groupings'!C9</f>
         <v>0</v>
       </c>
-      <c r="O23" s="107"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="4"/>
+      <c r="O23" s="152"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="3"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A24" s="96"/>
-      <c r="B24" s="97"/>
-      <c r="C24" s="98"/>
-      <c r="D24" s="102">
+      <c r="A24" s="77"/>
+      <c r="B24" s="78"/>
+      <c r="C24" s="79"/>
+      <c r="D24" s="70">
         <v>3</v>
       </c>
-      <c r="E24" s="103"/>
-      <c r="F24" s="104">
+      <c r="E24" s="71"/>
+      <c r="F24" s="68">
         <v>41560</v>
       </c>
-      <c r="G24" s="105"/>
-      <c r="H24" s="106">
+      <c r="G24" s="69"/>
+      <c r="H24" s="151">
         <f>'Family Income Groupings'!C4</f>
         <v>0</v>
       </c>
-      <c r="I24" s="106"/>
-      <c r="J24" s="102">
+      <c r="I24" s="151"/>
+      <c r="J24" s="70">
         <v>9</v>
       </c>
-      <c r="K24" s="103"/>
-      <c r="L24" s="104">
+      <c r="K24" s="71"/>
+      <c r="L24" s="68">
         <v>93400</v>
       </c>
-      <c r="M24" s="105"/>
-      <c r="N24" s="107">
+      <c r="M24" s="69"/>
+      <c r="N24" s="152">
         <f>'Family Income Groupings'!C10</f>
         <v>0</v>
       </c>
-      <c r="O24" s="107"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="4"/>
+      <c r="O24" s="152"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="3"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A25" s="96"/>
-      <c r="B25" s="97"/>
-      <c r="C25" s="98"/>
-      <c r="D25" s="102">
+      <c r="A25" s="77"/>
+      <c r="B25" s="78"/>
+      <c r="C25" s="79"/>
+      <c r="D25" s="70">
         <v>4</v>
       </c>
-      <c r="E25" s="103"/>
-      <c r="F25" s="104">
+      <c r="E25" s="71"/>
+      <c r="F25" s="68">
         <v>50200</v>
       </c>
-      <c r="G25" s="105"/>
-      <c r="H25" s="106">
+      <c r="G25" s="69"/>
+      <c r="H25" s="151">
         <f>'Family Income Groupings'!C5</f>
         <v>0</v>
       </c>
-      <c r="I25" s="106"/>
-      <c r="J25" s="102">
+      <c r="I25" s="151"/>
+      <c r="J25" s="70">
         <v>10</v>
       </c>
-      <c r="K25" s="103"/>
-      <c r="L25" s="104">
+      <c r="K25" s="71"/>
+      <c r="L25" s="68">
         <v>102040</v>
       </c>
-      <c r="M25" s="105"/>
-      <c r="N25" s="107">
+      <c r="M25" s="69"/>
+      <c r="N25" s="152">
         <f>'Family Income Groupings'!C11</f>
         <v>0</v>
       </c>
-      <c r="O25" s="107"/>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="4"/>
+      <c r="O25" s="152"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="3"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A26" s="96"/>
-      <c r="B26" s="97"/>
-      <c r="C26" s="98"/>
-      <c r="D26" s="102">
+      <c r="A26" s="77"/>
+      <c r="B26" s="78"/>
+      <c r="C26" s="79"/>
+      <c r="D26" s="70">
         <v>5</v>
       </c>
-      <c r="E26" s="103"/>
-      <c r="F26" s="104">
+      <c r="E26" s="71"/>
+      <c r="F26" s="68">
         <v>58840</v>
       </c>
-      <c r="G26" s="105"/>
-      <c r="H26" s="106">
+      <c r="G26" s="69"/>
+      <c r="H26" s="151">
         <f>'Family Income Groupings'!C6</f>
         <v>0</v>
       </c>
-      <c r="I26" s="106"/>
-      <c r="J26" s="102">
+      <c r="I26" s="151"/>
+      <c r="J26" s="70">
         <v>11</v>
       </c>
-      <c r="K26" s="103"/>
-      <c r="L26" s="104">
+      <c r="K26" s="71"/>
+      <c r="L26" s="68">
         <v>110680</v>
       </c>
-      <c r="M26" s="105"/>
-      <c r="N26" s="107">
+      <c r="M26" s="69"/>
+      <c r="N26" s="152">
         <f>'Family Income Groupings'!C12</f>
         <v>0</v>
       </c>
-      <c r="O26" s="107"/>
-      <c r="P26" s="3"/>
-      <c r="Q26" s="4"/>
+      <c r="O26" s="152"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="3"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A27" s="99"/>
-      <c r="B27" s="100"/>
-      <c r="C27" s="101"/>
-      <c r="D27" s="112">
+      <c r="A27" s="80"/>
+      <c r="B27" s="81"/>
+      <c r="C27" s="82"/>
+      <c r="D27" s="72">
         <v>6</v>
       </c>
-      <c r="E27" s="112"/>
-      <c r="F27" s="113">
+      <c r="E27" s="72"/>
+      <c r="F27" s="73">
         <v>67480</v>
       </c>
-      <c r="G27" s="113"/>
-      <c r="H27" s="106">
+      <c r="G27" s="73"/>
+      <c r="H27" s="151">
         <f>'Family Income Groupings'!C7</f>
         <v>0</v>
       </c>
-      <c r="I27" s="106"/>
-      <c r="J27" s="112">
+      <c r="I27" s="151"/>
+      <c r="J27" s="72">
         <v>12</v>
       </c>
-      <c r="K27" s="112"/>
-      <c r="L27" s="113">
+      <c r="K27" s="72"/>
+      <c r="L27" s="73">
         <v>119320</v>
       </c>
-      <c r="M27" s="113"/>
-      <c r="N27" s="107">
+      <c r="M27" s="73"/>
+      <c r="N27" s="152">
         <f>'Family Income Groupings'!C13</f>
         <v>0</v>
       </c>
-      <c r="O27" s="107"/>
-      <c r="P27" s="3"/>
-      <c r="Q27" s="4"/>
+      <c r="O27" s="152"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="3"/>
     </row>
     <row r="28" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="74"/>
-      <c r="B28" s="75"/>
-      <c r="C28" s="75"/>
-      <c r="D28" s="75"/>
-      <c r="E28" s="75"/>
-      <c r="F28" s="75"/>
-      <c r="G28" s="75"/>
-      <c r="H28" s="75"/>
-      <c r="I28" s="75"/>
-      <c r="J28" s="75"/>
-      <c r="K28" s="75"/>
-      <c r="L28" s="75"/>
-      <c r="M28" s="75"/>
-      <c r="N28" s="75"/>
-      <c r="O28" s="75"/>
-      <c r="P28" s="75"/>
-      <c r="Q28" s="76"/>
+      <c r="A28" s="62"/>
+      <c r="B28" s="63"/>
+      <c r="C28" s="63"/>
+      <c r="D28" s="63"/>
+      <c r="E28" s="63"/>
+      <c r="F28" s="63"/>
+      <c r="G28" s="63"/>
+      <c r="H28" s="63"/>
+      <c r="I28" s="63"/>
+      <c r="J28" s="63"/>
+      <c r="K28" s="63"/>
+      <c r="L28" s="63"/>
+      <c r="M28" s="63"/>
+      <c r="N28" s="63"/>
+      <c r="O28" s="63"/>
+      <c r="P28" s="63"/>
+      <c r="Q28" s="64"/>
     </row>
     <row r="29" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="52" t="s">
+      <c r="A29" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="53"/>
-      <c r="C29" s="53"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="53"/>
-      <c r="G29" s="53"/>
-      <c r="H29" s="53"/>
-      <c r="I29" s="53"/>
-      <c r="J29" s="53"/>
-      <c r="K29" s="53"/>
-      <c r="L29" s="53"/>
-      <c r="M29" s="53"/>
-      <c r="N29" s="53"/>
-      <c r="O29" s="54"/>
-      <c r="P29" s="5"/>
-      <c r="Q29" s="8"/>
+      <c r="B29" s="66"/>
+      <c r="C29" s="66"/>
+      <c r="D29" s="66"/>
+      <c r="E29" s="66"/>
+      <c r="F29" s="66"/>
+      <c r="G29" s="66"/>
+      <c r="H29" s="66"/>
+      <c r="I29" s="66"/>
+      <c r="J29" s="66"/>
+      <c r="K29" s="66"/>
+      <c r="L29" s="66"/>
+      <c r="M29" s="66"/>
+      <c r="N29" s="66"/>
+      <c r="O29" s="67"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="7"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A30" s="55"/>
-      <c r="B30" s="56"/>
-      <c r="C30" s="108"/>
-      <c r="D30" s="59"/>
-      <c r="E30" s="61"/>
-      <c r="F30" s="60" t="s">
+      <c r="A30" s="117"/>
+      <c r="B30" s="118"/>
+      <c r="C30" s="127"/>
+      <c r="D30" s="119"/>
+      <c r="E30" s="121"/>
+      <c r="F30" s="120" t="s">
         <v>19</v>
       </c>
-      <c r="G30" s="61"/>
-      <c r="H30" s="59" t="s">
+      <c r="G30" s="121"/>
+      <c r="H30" s="119" t="s">
         <v>20</v>
       </c>
-      <c r="I30" s="60"/>
-      <c r="J30" s="59" t="s">
+      <c r="I30" s="120"/>
+      <c r="J30" s="119" t="s">
         <v>21</v>
       </c>
-      <c r="K30" s="61"/>
-      <c r="L30" s="60" t="s">
+      <c r="K30" s="121"/>
+      <c r="L30" s="120" t="s">
         <v>22</v>
       </c>
-      <c r="M30" s="61"/>
-      <c r="N30" s="59" t="s">
+      <c r="M30" s="121"/>
+      <c r="N30" s="119" t="s">
         <v>23</v>
       </c>
-      <c r="O30" s="61"/>
-      <c r="P30" s="3"/>
-      <c r="Q30" s="4"/>
+      <c r="O30" s="121"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="3"/>
     </row>
     <row r="31" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="109"/>
-      <c r="B31" s="110"/>
-      <c r="C31" s="111"/>
-      <c r="D31" s="114"/>
-      <c r="E31" s="115"/>
-      <c r="F31" s="116"/>
-      <c r="G31" s="115"/>
-      <c r="H31" s="114"/>
-      <c r="I31" s="116"/>
-      <c r="J31" s="114"/>
-      <c r="K31" s="115"/>
-      <c r="L31" s="116"/>
-      <c r="M31" s="115"/>
-      <c r="N31" s="114"/>
-      <c r="O31" s="115"/>
-      <c r="P31" s="3"/>
-      <c r="Q31" s="4"/>
+      <c r="A31" s="128"/>
+      <c r="B31" s="129"/>
+      <c r="C31" s="130"/>
+      <c r="D31" s="131"/>
+      <c r="E31" s="132"/>
+      <c r="F31" s="133"/>
+      <c r="G31" s="132"/>
+      <c r="H31" s="131"/>
+      <c r="I31" s="133"/>
+      <c r="J31" s="131"/>
+      <c r="K31" s="132"/>
+      <c r="L31" s="133"/>
+      <c r="M31" s="132"/>
+      <c r="N31" s="131"/>
+      <c r="O31" s="132"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="3"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A32" s="126" t="s">
+      <c r="A32" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="127"/>
-      <c r="C32" s="128"/>
-      <c r="D32" s="117"/>
-      <c r="E32" s="118"/>
-      <c r="F32" s="129">
+      <c r="B32" s="57"/>
+      <c r="C32" s="58"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="49">
         <f>IFERROR((G5*D13)*D16,0)+IFERROR((G5*D14)*D17,0)+IFERROR((G5*E13)*E16,0)+IFERROR((G5*E14)*E17,0)</f>
         <v>0</v>
       </c>
-      <c r="G32" s="130"/>
-      <c r="H32" s="131"/>
-      <c r="I32" s="132"/>
-      <c r="J32" s="133"/>
-      <c r="K32" s="132"/>
-      <c r="L32" s="133"/>
-      <c r="M32" s="132"/>
-      <c r="N32" s="117"/>
-      <c r="O32" s="118"/>
-      <c r="P32" s="9"/>
-      <c r="Q32" s="10"/>
+      <c r="G32" s="50"/>
+      <c r="H32" s="59"/>
+      <c r="I32" s="60"/>
+      <c r="J32" s="61"/>
+      <c r="K32" s="60"/>
+      <c r="L32" s="61"/>
+      <c r="M32" s="60"/>
+      <c r="N32" s="44"/>
+      <c r="O32" s="45"/>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="9"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A33" s="119" t="s">
+      <c r="A33" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="B33" s="120"/>
-      <c r="C33" s="121"/>
-      <c r="D33" s="117"/>
-      <c r="E33" s="118"/>
-      <c r="F33" s="122">
+      <c r="B33" s="47"/>
+      <c r="C33" s="48"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="54">
         <f>IFERROR((G5*F13)*F16,0)+IFERROR((G5*F14)*F17,0)+IFERROR((G5*G13)*G16,0)+IFERROR((G5*G14)*G17,0)</f>
         <v>0</v>
       </c>
-      <c r="G33" s="123"/>
-      <c r="H33" s="85"/>
-      <c r="I33" s="124"/>
-      <c r="J33" s="125"/>
-      <c r="K33" s="124"/>
-      <c r="L33" s="125"/>
-      <c r="M33" s="124"/>
-      <c r="N33" s="117"/>
-      <c r="O33" s="118"/>
-      <c r="P33" s="11"/>
-      <c r="Q33" s="12"/>
+      <c r="G33" s="55"/>
+      <c r="H33" s="51"/>
+      <c r="I33" s="52"/>
+      <c r="J33" s="53"/>
+      <c r="K33" s="52"/>
+      <c r="L33" s="53"/>
+      <c r="M33" s="52"/>
+      <c r="N33" s="44"/>
+      <c r="O33" s="45"/>
+      <c r="P33" s="10"/>
+      <c r="Q33" s="11"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A34" s="119" t="s">
+      <c r="A34" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="120"/>
-      <c r="C34" s="121"/>
-      <c r="D34" s="117"/>
-      <c r="E34" s="118"/>
-      <c r="F34" s="129">
+      <c r="B34" s="47"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="49">
         <f>IFERROR((G5*H13)*H16,0)+IFERROR((G5*I13)*I16,0)+IFERROR((G5*J13)*J16,0)</f>
         <v>0</v>
       </c>
-      <c r="G34" s="130"/>
-      <c r="H34" s="85"/>
-      <c r="I34" s="124"/>
-      <c r="J34" s="125"/>
-      <c r="K34" s="124"/>
-      <c r="L34" s="125"/>
-      <c r="M34" s="124"/>
-      <c r="N34" s="117"/>
-      <c r="O34" s="118"/>
-      <c r="P34" s="11"/>
-      <c r="Q34" s="12"/>
+      <c r="G34" s="50"/>
+      <c r="H34" s="51"/>
+      <c r="I34" s="52"/>
+      <c r="J34" s="53"/>
+      <c r="K34" s="52"/>
+      <c r="L34" s="53"/>
+      <c r="M34" s="52"/>
+      <c r="N34" s="44"/>
+      <c r="O34" s="45"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="11"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A35" s="119" t="s">
+      <c r="A35" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="120"/>
-      <c r="C35" s="121"/>
-      <c r="D35" s="117"/>
-      <c r="E35" s="118"/>
-      <c r="F35" s="129">
+      <c r="B35" s="47"/>
+      <c r="C35" s="48"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="49">
         <f>IFERROR((G5*K13)*K17,0)+IFERROR((G5*L13)*L17,0)+IFERROR((G5*M13)*M17,0)</f>
         <v>0</v>
       </c>
-      <c r="G35" s="130"/>
-      <c r="H35" s="85"/>
-      <c r="I35" s="124"/>
-      <c r="J35" s="125"/>
-      <c r="K35" s="124"/>
-      <c r="L35" s="125"/>
-      <c r="M35" s="124"/>
-      <c r="N35" s="117"/>
-      <c r="O35" s="118"/>
-      <c r="P35" s="11"/>
-      <c r="Q35" s="12"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="51"/>
+      <c r="I35" s="52"/>
+      <c r="J35" s="53"/>
+      <c r="K35" s="52"/>
+      <c r="L35" s="53"/>
+      <c r="M35" s="52"/>
+      <c r="N35" s="44"/>
+      <c r="O35" s="45"/>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="11"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A36" s="119" t="s">
+      <c r="A36" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="B36" s="120"/>
-      <c r="C36" s="121"/>
-      <c r="D36" s="117"/>
-      <c r="E36" s="118"/>
-      <c r="F36" s="129">
+      <c r="B36" s="47"/>
+      <c r="C36" s="48"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="49">
         <f>IFERROR((G5*N13)*N16,0)+IFERROR((G5*N14)*N17,0)+IFERROR((G5*O13)*O16,0)+IFERROR((G5*O14)*O17,0)</f>
         <v>0</v>
       </c>
-      <c r="G36" s="130"/>
-      <c r="H36" s="85"/>
-      <c r="I36" s="124"/>
-      <c r="J36" s="125"/>
-      <c r="K36" s="124"/>
-      <c r="L36" s="125"/>
-      <c r="M36" s="124"/>
-      <c r="N36" s="117"/>
-      <c r="O36" s="118"/>
-      <c r="P36" s="11"/>
-      <c r="Q36" s="12"/>
+      <c r="G36" s="50"/>
+      <c r="H36" s="51"/>
+      <c r="I36" s="52"/>
+      <c r="J36" s="53"/>
+      <c r="K36" s="52"/>
+      <c r="L36" s="53"/>
+      <c r="M36" s="52"/>
+      <c r="N36" s="44"/>
+      <c r="O36" s="45"/>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="11"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A37" s="119" t="s">
+      <c r="A37" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="B37" s="120"/>
-      <c r="C37" s="121"/>
-      <c r="D37" s="117"/>
-      <c r="E37" s="118"/>
-      <c r="F37" s="129">
+      <c r="B37" s="47"/>
+      <c r="C37" s="48"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="49">
         <f>IFERROR((G5*P13)*P16,0)+IFERROR((G5*P14)*P17,0)+IFERROR((G5*Q13)*Q16,0)+IFERROR((G5*Q14)*Q17,0)</f>
         <v>0</v>
       </c>
-      <c r="G37" s="130"/>
-      <c r="H37" s="85"/>
-      <c r="I37" s="124"/>
-      <c r="J37" s="125"/>
-      <c r="K37" s="124"/>
-      <c r="L37" s="125"/>
-      <c r="M37" s="124"/>
-      <c r="N37" s="117"/>
-      <c r="O37" s="118"/>
-      <c r="P37" s="11"/>
-      <c r="Q37" s="12"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="51"/>
+      <c r="I37" s="52"/>
+      <c r="J37" s="53"/>
+      <c r="K37" s="52"/>
+      <c r="L37" s="53"/>
+      <c r="M37" s="52"/>
+      <c r="N37" s="44"/>
+      <c r="O37" s="45"/>
+      <c r="P37" s="10"/>
+      <c r="Q37" s="11"/>
     </row>
     <row r="38" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="152" t="s">
+      <c r="A38" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="B38" s="153"/>
-      <c r="C38" s="154"/>
-      <c r="D38" s="155"/>
-      <c r="E38" s="156"/>
-      <c r="F38" s="157">
+      <c r="B38" s="38"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="41"/>
+      <c r="F38" s="42">
         <f>SUM(F32:G37)</f>
         <v>0</v>
       </c>
-      <c r="G38" s="158"/>
-      <c r="H38" s="159">
+      <c r="G38" s="43"/>
+      <c r="H38" s="153">
         <f>'Other Details'!D2</f>
         <v>0</v>
       </c>
-      <c r="I38" s="160"/>
-      <c r="J38" s="161">
+      <c r="I38" s="154"/>
+      <c r="J38" s="155">
         <f>'Other Details'!E2</f>
         <v>0</v>
       </c>
-      <c r="K38" s="162"/>
-      <c r="L38" s="163">
+      <c r="K38" s="156"/>
+      <c r="L38" s="157">
         <f>'Other Details'!F2</f>
         <v>0</v>
       </c>
-      <c r="M38" s="160"/>
-      <c r="N38" s="140">
+      <c r="M38" s="154"/>
+      <c r="N38" s="28">
         <f t="shared" ref="N38" si="0">SUM(F38,H38,L38)</f>
         <v>0</v>
       </c>
-      <c r="O38" s="141"/>
-      <c r="P38" s="11"/>
-      <c r="Q38" s="12"/>
+      <c r="O38" s="29"/>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="11"/>
     </row>
     <row r="39" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="142"/>
-      <c r="B39" s="143"/>
-      <c r="C39" s="143"/>
-      <c r="D39" s="143"/>
-      <c r="E39" s="143"/>
-      <c r="F39" s="143"/>
-      <c r="G39" s="143"/>
-      <c r="H39" s="143"/>
-      <c r="I39" s="143"/>
-      <c r="J39" s="143"/>
-      <c r="K39" s="143"/>
-      <c r="L39" s="143"/>
-      <c r="M39" s="143"/>
-      <c r="N39" s="5"/>
-      <c r="O39" s="5"/>
-      <c r="P39" s="5"/>
-      <c r="Q39" s="8"/>
+      <c r="A39" s="30"/>
+      <c r="B39" s="31"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="31"/>
+      <c r="H39" s="31"/>
+      <c r="I39" s="31"/>
+      <c r="J39" s="31"/>
+      <c r="K39" s="31"/>
+      <c r="L39" s="31"/>
+      <c r="M39" s="31"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="4"/>
+      <c r="Q39" s="7"/>
     </row>
     <row r="40" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="144" t="s">
+      <c r="A40" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="145"/>
-      <c r="C40" s="145"/>
-      <c r="D40" s="145"/>
-      <c r="E40" s="145"/>
-      <c r="F40" s="145"/>
-      <c r="G40" s="145"/>
-      <c r="H40" s="145"/>
-      <c r="I40" s="145"/>
-      <c r="J40" s="145"/>
-      <c r="K40" s="145"/>
-      <c r="L40" s="145"/>
-      <c r="M40" s="146"/>
-      <c r="Q40" s="2"/>
+      <c r="B40" s="33"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="33"/>
+      <c r="I40" s="33"/>
+      <c r="J40" s="33"/>
+      <c r="K40" s="33"/>
+      <c r="L40" s="33"/>
+      <c r="M40" s="34"/>
+      <c r="Q40" s="1"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A41" s="147" t="s">
+      <c r="A41" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B41" s="148"/>
-      <c r="C41" s="149" t="s">
+      <c r="B41" s="36"/>
+      <c r="C41" s="158" t="s">
         <v>35</v>
       </c>
-      <c r="D41" s="150"/>
-      <c r="E41" s="150"/>
-      <c r="F41" s="150"/>
-      <c r="G41" s="150"/>
-      <c r="H41" s="150"/>
-      <c r="I41" s="150"/>
-      <c r="J41" s="150"/>
-      <c r="K41" s="150"/>
-      <c r="L41" s="150"/>
-      <c r="M41" s="151"/>
-      <c r="N41" s="23"/>
-      <c r="O41" s="23"/>
-      <c r="P41" s="23"/>
-      <c r="Q41" s="24"/>
+      <c r="D41" s="159"/>
+      <c r="E41" s="159"/>
+      <c r="F41" s="159"/>
+      <c r="G41" s="159"/>
+      <c r="H41" s="159"/>
+      <c r="I41" s="159"/>
+      <c r="J41" s="159"/>
+      <c r="K41" s="159"/>
+      <c r="L41" s="159"/>
+      <c r="M41" s="160"/>
+      <c r="N41" s="20"/>
+      <c r="O41" s="20"/>
+      <c r="P41" s="20"/>
+      <c r="Q41" s="21"/>
     </row>
     <row r="42" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="134" t="s">
+      <c r="A42" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="135"/>
-      <c r="C42" s="136">
+      <c r="B42" s="26"/>
+      <c r="C42" s="161">
         <f>'Other Details'!G2</f>
         <v>0</v>
       </c>
-      <c r="D42" s="137"/>
-      <c r="E42" s="137"/>
-      <c r="F42" s="137"/>
-      <c r="G42" s="137"/>
-      <c r="H42" s="137"/>
-      <c r="I42" s="137"/>
-      <c r="J42" s="137"/>
-      <c r="K42" s="137"/>
-      <c r="L42" s="137"/>
-      <c r="M42" s="138"/>
-      <c r="N42" s="13"/>
-      <c r="O42" s="13"/>
-      <c r="P42" s="13"/>
-      <c r="Q42" s="14"/>
+      <c r="D42" s="162"/>
+      <c r="E42" s="162"/>
+      <c r="F42" s="162"/>
+      <c r="G42" s="162"/>
+      <c r="H42" s="162"/>
+      <c r="I42" s="162"/>
+      <c r="J42" s="162"/>
+      <c r="K42" s="162"/>
+      <c r="L42" s="162"/>
+      <c r="M42" s="163"/>
+      <c r="N42" s="12"/>
+      <c r="O42" s="12"/>
+      <c r="P42" s="12"/>
+      <c r="Q42" s="13"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A43" s="139" t="s">
+      <c r="A43" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B43" s="139"/>
-      <c r="C43" s="139"/>
-      <c r="D43" s="139"/>
-      <c r="E43" s="139"/>
-      <c r="F43" s="139"/>
-      <c r="G43" s="139"/>
-      <c r="H43" s="139"/>
-      <c r="I43" s="139"/>
-      <c r="J43" s="139"/>
-      <c r="K43" s="139"/>
-      <c r="L43" s="139"/>
-      <c r="M43" s="139"/>
-      <c r="N43" s="139"/>
-      <c r="O43" s="139"/>
-      <c r="P43" s="139"/>
-      <c r="Q43" s="139"/>
+      <c r="B43" s="27"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="27"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
+      <c r="K43" s="27"/>
+      <c r="L43" s="27"/>
+      <c r="M43" s="27"/>
+      <c r="N43" s="27"/>
+      <c r="O43" s="27"/>
+      <c r="P43" s="27"/>
+      <c r="Q43" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="142">
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C42:M42"/>
-    <mergeCell ref="A43:Q43"/>
-    <mergeCell ref="N38:O38"/>
-    <mergeCell ref="A39:M39"/>
-    <mergeCell ref="A40:M40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:M41"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="L38:M38"/>
-    <mergeCell ref="N36:O36"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="L37:M37"/>
-    <mergeCell ref="N37:O37"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="J36:K36"/>
-    <mergeCell ref="L36:M36"/>
-    <mergeCell ref="N34:O34"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="J35:K35"/>
-    <mergeCell ref="L35:M35"/>
-    <mergeCell ref="N35:O35"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="L34:M34"/>
-    <mergeCell ref="N32:O32"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="N33:O33"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="A28:Q28"/>
-    <mergeCell ref="A29:O29"/>
-    <mergeCell ref="A30:C31"/>
-    <mergeCell ref="D30:E31"/>
-    <mergeCell ref="F30:G31"/>
-    <mergeCell ref="H30:I31"/>
-    <mergeCell ref="J30:K31"/>
-    <mergeCell ref="L30:M31"/>
-    <mergeCell ref="N30:O31"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="H2:Q2"/>
+    <mergeCell ref="A3:Q3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="G4:M4"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="G5:M5"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="A6:Q6"/>
+    <mergeCell ref="A7:Q7"/>
+    <mergeCell ref="A8:C9"/>
+    <mergeCell ref="D8:G9"/>
+    <mergeCell ref="H8:M9"/>
+    <mergeCell ref="N8:Q9"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="H17:M17"/>
+    <mergeCell ref="A18:Q18"/>
+    <mergeCell ref="A19:O19"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:Q12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="H14:M14"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="N10:O10"/>
     <mergeCell ref="N20:O21"/>
     <mergeCell ref="A22:C27"/>
     <mergeCell ref="D22:E22"/>
@@ -3060,42 +3008,94 @@
     <mergeCell ref="N25:O25"/>
     <mergeCell ref="H23:I23"/>
     <mergeCell ref="J23:K23"/>
-    <mergeCell ref="A18:Q18"/>
-    <mergeCell ref="A19:O19"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A12:Q12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="H14:M14"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="A6:Q6"/>
-    <mergeCell ref="A7:Q7"/>
-    <mergeCell ref="A8:C9"/>
-    <mergeCell ref="D8:G9"/>
-    <mergeCell ref="H8:M9"/>
-    <mergeCell ref="N8:Q9"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="H17:M17"/>
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="H2:Q2"/>
-    <mergeCell ref="A3:Q3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="G4:M4"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="G5:M5"/>
-    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="A28:Q28"/>
+    <mergeCell ref="A29:O29"/>
+    <mergeCell ref="A30:C31"/>
+    <mergeCell ref="D30:E31"/>
+    <mergeCell ref="F30:G31"/>
+    <mergeCell ref="H30:I31"/>
+    <mergeCell ref="J30:K31"/>
+    <mergeCell ref="L30:M31"/>
+    <mergeCell ref="N30:O31"/>
+    <mergeCell ref="N32:O32"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="N34:O34"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="N35:O35"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="L37:M37"/>
+    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="L36:M36"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:M42"/>
+    <mergeCell ref="A43:Q43"/>
+    <mergeCell ref="N38:O38"/>
+    <mergeCell ref="A39:M39"/>
+    <mergeCell ref="A40:M40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="C41:M41"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="L38:M38"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="79" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="89" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
@@ -3121,20 +3121,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="26"/>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
+      <c r="A1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3153,9 +3153,9 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="26"/>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
+      <c r="A1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3174,13 +3174,13 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="26"/>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="A1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3199,13 +3199,13 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="26"/>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="A1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>